<commit_message>
W306 H0600 - Acount & Acount (lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\共用\Github\Family\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="419" yWindow="105" windowWidth="16979" windowHeight="6336"/>
+    <workbookView xWindow="420" yWindow="110" windowWidth="16980" windowHeight="6340"/>
   </bookViews>
   <sheets>
     <sheet name="金融簡易版" sheetId="4" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <author>Bali-ThinkPad</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -587,15 +592,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W304 H0900</t>
+    <t>台新Richar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>812</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敦南(0023)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2888-10-0785134-0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2888-10-0785170-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W306 H0600</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -685,6 +710,14 @@
       <family val="3"/>
       <charset val="136"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -805,12 +838,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -820,43 +852,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -865,6 +866,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -873,6 +910,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -919,7 +964,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,9 +996,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -985,6 +1031,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1160,416 +1207,487 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:G22"/>
+  <dimension ref="A2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.05" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.25" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="16.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.26953125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="16.399999999999999">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26" t="s">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.35">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.35">
+      <c r="A4" s="15"/>
+      <c r="B4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A6" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A7" s="20"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A9" s="20"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A10" s="20"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="5">
+        <v>812</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A11" s="20"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5">
+        <v>812</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="5">
+        <v>822</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A14" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5">
+        <v>822</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:7" ht="16.399999999999999">
-      <c r="A3" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.399999999999999">
-      <c r="A4" s="23"/>
-      <c r="B4" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="16.399999999999999">
-      <c r="A6" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="D16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A18" s="27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="16.399999999999999">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16.399999999999999">
-      <c r="A8" s="13"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="B18" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5">
+        <v>822</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.399999999999999">
-      <c r="A9" s="13"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16.399999999999999">
-      <c r="A10" s="13"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="6">
-        <v>812</v>
-      </c>
-      <c r="E10" s="4" t="s">
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A19" s="27"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A20" s="27"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A22" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5">
+        <v>822</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.399999999999999">
-      <c r="A11" s="13"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="6">
-        <v>812</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="3">
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16.399999999999999">
-      <c r="A12" s="13"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="6">
-        <v>822</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="16.399999999999999">
-      <c r="A14" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16.399999999999999">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="6">
-        <v>822</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.399999999999999">
-      <c r="A17" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="6">
-        <v>822</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="16.399999999999999">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="16.399999999999999">
-      <c r="A20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="6">
-        <v>822</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="16.399999999999999">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="B6:B12"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" display="中國信託"/>
-    <hyperlink ref="C15" r:id="rId2"/>
-    <hyperlink ref="C17" r:id="rId3"/>
-    <hyperlink ref="C20" r:id="rId4"/>
-    <hyperlink ref="C7" r:id="rId5" display="台北富邦銀行"/>
-    <hyperlink ref="C14" r:id="rId6"/>
-    <hyperlink ref="C6" r:id="rId7" display="台灣營行"/>
-    <hyperlink ref="C10" r:id="rId8" display="台新銀行"/>
-    <hyperlink ref="C8" r:id="rId9" display="國泰世華"/>
-    <hyperlink ref="C9" r:id="rId10"/>
+    <hyperlink ref="C18" r:id="rId2"/>
+    <hyperlink ref="C22" r:id="rId3"/>
+    <hyperlink ref="C7" r:id="rId4" display="台北富邦銀行"/>
+    <hyperlink ref="C14" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6" display="台灣營行"/>
+    <hyperlink ref="C10" r:id="rId7" display="台新銀行"/>
+    <hyperlink ref="C8" r:id="rId8" display="國泰世華"/>
+    <hyperlink ref="C9" r:id="rId9"/>
+    <hyperlink ref="C15" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId11"/>

</xml_diff>

<commit_message>
W311 H1400 Account & Account (lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\共用\Github\Family\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="110" windowWidth="16980" windowHeight="6340"/>
+    <workbookView xWindow="419" yWindow="105" windowWidth="16979" windowHeight="6336"/>
   </bookViews>
   <sheets>
     <sheet name="金融簡易版" sheetId="4" r:id="rId1"/>
@@ -24,7 +19,7 @@
     <author>Bali-ThinkPad</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0">
+    <comment ref="F11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
+    <comment ref="C12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -228,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -307,20 +302,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>曾辰哲</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">406-53-4465906         </t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -612,15 +593,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W306 H0600</t>
+    <t>曾辰哲</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>W311 H1400</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -727,7 +712,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -827,6 +812,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -838,7 +847,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -866,6 +875,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -873,35 +908,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -964,7 +1000,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -996,10 +1032,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1031,7 +1066,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1207,36 +1241,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:G27"/>
+  <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.05" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="16.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.90625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.26953125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.90625" style="1"/>
+    <col min="2" max="2" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.25" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="16.399999999999999">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>59</v>
@@ -1245,134 +1279,134 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>52</v>
+    <row r="3" spans="1:10" ht="16.399999999999999">
+      <c r="A3" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
+      <c r="C3" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="1:10" ht="16.399999999999999">
+      <c r="A4" s="29"/>
       <c r="B4" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A6" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="21" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:10" ht="16.399999999999999">
+      <c r="A6" s="32" t="s">
         <v>43</v>
       </c>
+      <c r="B6" s="27" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A7" s="20"/>
-      <c r="B7" s="22"/>
+    <row r="7" spans="1:10" ht="16.399999999999999">
+      <c r="A7" s="33"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A8" s="20"/>
-      <c r="B8" s="22"/>
+    <row r="8" spans="1:10" ht="16.399999999999999">
+      <c r="A8" s="33"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A9" s="20"/>
-      <c r="B9" s="22"/>
+    <row r="9" spans="1:10" ht="16.399999999999999">
+      <c r="A9" s="33"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A10" s="20"/>
-      <c r="B10" s="22"/>
+    <row r="10" spans="1:10" ht="16.399999999999999">
+      <c r="A10" s="33"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5">
         <v>812</v>
@@ -1381,317 +1415,380 @@
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A11" s="20"/>
-      <c r="B11" s="22"/>
+    <row r="11" spans="1:10" ht="16.399999999999999">
+      <c r="A11" s="33"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="5">
         <v>812</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A12" s="20"/>
-      <c r="B12" s="22"/>
+    <row r="12" spans="1:10" ht="16.399999999999999">
+      <c r="A12" s="34"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="5">
         <v>822</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A14" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="21" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.399999999999999">
+      <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
+      <c r="B14" s="27" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A15" s="20"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="6" t="s">
+    <row r="15" spans="1:10" ht="16.399999999999999">
+      <c r="A15" s="33"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="5">
+        <v>812</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="16.399999999999999">
+      <c r="A16" s="33"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.399999999999999">
+      <c r="A17" s="33"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D17" s="5">
         <v>822</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E17" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="F17" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A16" s="20"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A18" s="27" t="s">
+      <c r="G17" s="2">
         <v>12</v>
       </c>
-      <c r="B18" s="25" t="s">
+    </row>
+    <row r="18" spans="1:7" ht="16.399999999999999">
+      <c r="A18" s="34"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="1:7" ht="16.399999999999999">
+      <c r="A20" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5">
-        <v>822</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="G19" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="G20" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-    </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A22" s="25" t="s">
+    <row r="21" spans="1:7" ht="16.399999999999999">
+      <c r="A21" s="37"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="5">
+        <v>812</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="16.399999999999999">
+      <c r="A22" s="37"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16.399999999999999">
+      <c r="A23" s="37"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="5">
+        <v>822</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="38"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="1:7" ht="16.399999999999999">
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="1:7" ht="16.399999999999999">
+      <c r="A26" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16.399999999999999">
+      <c r="A27" s="40"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="5">
+        <v>812</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="16.399999999999999">
+      <c r="A28" s="40"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="16.399999999999999">
+      <c r="A29" s="40"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D29" s="5">
         <v>822</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E29" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F29" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G29" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
+    <row r="30" spans="1:7">
+      <c r="A30" s="41"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
+  <mergeCells count="14">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="B6:B12"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" display="中國信託"/>
-    <hyperlink ref="C18" r:id="rId2"/>
-    <hyperlink ref="C22" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4" display="台北富邦銀行"/>
-    <hyperlink ref="C14" r:id="rId5"/>
-    <hyperlink ref="C6" r:id="rId6" display="台灣營行"/>
-    <hyperlink ref="C10" r:id="rId7" display="台新銀行"/>
-    <hyperlink ref="C8" r:id="rId8" display="國泰世華"/>
-    <hyperlink ref="C9" r:id="rId9"/>
-    <hyperlink ref="C15" r:id="rId10"/>
+    <hyperlink ref="C6" r:id="rId2" display="台灣營行"/>
+    <hyperlink ref="C14" r:id="rId3"/>
+    <hyperlink ref="C10" r:id="rId4" display="台新銀行"/>
+    <hyperlink ref="C8" r:id="rId5" display="國泰世華"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="C17" r:id="rId7"/>
+    <hyperlink ref="C23" r:id="rId8"/>
+    <hyperlink ref="C29" r:id="rId9"/>
+    <hyperlink ref="C15" r:id="rId10" display="台新銀行"/>
+    <hyperlink ref="C21" r:id="rId11" display="台新銀行"/>
+    <hyperlink ref="C27" r:id="rId12" display="台新銀行"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId13"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId12"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
W312 H0800- Account (lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -597,7 +597,15 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>W311 H1400</t>
+    <t>2888-10-0786338-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敦南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W312 H0800</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -847,7 +855,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -882,25 +890,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -908,6 +898,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -917,6 +908,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,15 +946,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1248,10 +1257,10 @@
   <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.05" outlineLevelCol="1"/>
@@ -1273,27 +1282,27 @@
         <v>52</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="16.399999999999999">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:10" ht="16.399999999999999">
-      <c r="A4" s="29"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="11" t="s">
         <v>49</v>
       </c>
@@ -1314,8 +1323,8 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
@@ -1323,10 +1332,10 @@
       <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:10" ht="16.399999999999999">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1346,8 +1355,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.399999999999999">
-      <c r="A7" s="33"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="9" t="s">
         <v>37</v>
       </c>
@@ -1365,8 +1374,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.399999999999999">
-      <c r="A8" s="33"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="9" t="s">
         <v>34</v>
       </c>
@@ -1384,8 +1393,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.399999999999999">
-      <c r="A9" s="33"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="8" t="s">
         <v>30</v>
       </c>
@@ -1403,8 +1412,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.399999999999999">
-      <c r="A10" s="33"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="9" t="s">
         <v>26</v>
       </c>
@@ -1422,8 +1431,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="16.399999999999999">
-      <c r="A11" s="33"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="8" t="s">
         <v>24</v>
       </c>
@@ -1441,8 +1450,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.399999999999999">
-      <c r="A12" s="34"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1460,8 +1469,8 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -1469,10 +1478,10 @@
       <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:10" ht="16.399999999999999">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1492,21 +1501,22 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="16.399999999999999">
-      <c r="A15" s="33"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="5">
         <v>812</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="19"/>
+      <c r="E15" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="16.399999999999999">
-      <c r="A16" s="33"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="16" t="s">
         <v>53</v>
       </c>
@@ -1514,15 +1524,19 @@
         <v>54</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="2">
+        <v>12</v>
+      </c>
       <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="16.399999999999999">
-      <c r="A17" s="33"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
@@ -1540,8 +1554,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.399999999999999">
-      <c r="A18" s="34"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="16"/>
       <c r="D18" s="5"/>
       <c r="E18" s="4"/>
@@ -1558,10 +1572,10 @@
       <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:7" ht="16.399999999999999">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1581,8 +1595,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.399999999999999">
-      <c r="A21" s="37"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="9" t="s">
         <v>26</v>
       </c>
@@ -1594,8 +1608,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="16.399999999999999">
-      <c r="A22" s="37"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="16" t="s">
         <v>53</v>
       </c>
@@ -1603,7 +1617,7 @@
         <v>54</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>56</v>
@@ -1613,8 +1627,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="16.399999999999999">
-      <c r="A23" s="37"/>
-      <c r="B23" s="24"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
@@ -1632,8 +1646,8 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="38"/>
-      <c r="B24" s="24"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -1641,19 +1655,19 @@
       <c r="G24" s="21"/>
     </row>
     <row r="25" spans="1:7" ht="16.399999999999999">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="16.399999999999999">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -1673,8 +1687,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="16.399999999999999">
-      <c r="A27" s="40"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="9" t="s">
         <v>26</v>
       </c>
@@ -1686,8 +1700,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="16.399999999999999">
-      <c r="A28" s="40"/>
-      <c r="B28" s="24"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="16" t="s">
         <v>53</v>
       </c>
@@ -1705,8 +1719,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="16.399999999999999">
-      <c r="A29" s="40"/>
-      <c r="B29" s="24"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="6" t="s">
         <v>6</v>
       </c>
@@ -1724,8 +1738,8 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="41"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="6"/>
       <c r="D30" s="5"/>
       <c r="E30" s="15"/>
@@ -1756,11 +1770,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:B12"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="B26:B30"/>
@@ -1770,6 +1779,11 @@
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
W312 H0830- Account & Account (lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -218,12 +218,47 @@
         </r>
       </text>
     </comment>
+    <comment ref="C28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t xml:space="preserve">網路只可設定非約定
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -605,7 +640,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W312 H0800</t>
+    <t>玉山綜存</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>808</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0163-979-125049</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>W312 H0830</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>永豐銀行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>807</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北投</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110-018-0012788-3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -855,7 +918,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -891,6 +954,53 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -898,54 +1008,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1254,13 +1325,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:J33"/>
+  <dimension ref="A2:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.05" outlineLevelCol="1"/>
@@ -1275,34 +1346,34 @@
     <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="16.399999999999999">
+    <row r="2" spans="1:7" ht="16.399999999999999">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:10" ht="16.399999999999999">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:7" ht="16.399999999999999">
+      <c r="A3" s="40" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-    </row>
-    <row r="4" spans="1:10" ht="16.399999999999999">
-      <c r="A4" s="23"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.399999999999999">
+      <c r="A4" s="40"/>
       <c r="B4" s="11" t="s">
         <v>49</v>
       </c>
@@ -1322,20 +1393,20 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="1:10" ht="16.399999999999999">
-      <c r="A6" s="27" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.399999999999999">
+      <c r="A6" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="35" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1354,9 +1425,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16.399999999999999">
-      <c r="A7" s="28"/>
-      <c r="B7" s="31"/>
+    <row r="7" spans="1:7" ht="16.399999999999999">
+      <c r="A7" s="33"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="9" t="s">
         <v>37</v>
       </c>
@@ -1373,9 +1444,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16.399999999999999">
-      <c r="A8" s="28"/>
-      <c r="B8" s="31"/>
+    <row r="8" spans="1:7" ht="16.399999999999999">
+      <c r="A8" s="33"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="9" t="s">
         <v>34</v>
       </c>
@@ -1392,9 +1463,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="16.399999999999999">
-      <c r="A9" s="28"/>
-      <c r="B9" s="31"/>
+    <row r="9" spans="1:7" ht="16.399999999999999">
+      <c r="A9" s="33"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="8" t="s">
         <v>30</v>
       </c>
@@ -1411,9 +1482,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16.399999999999999">
-      <c r="A10" s="28"/>
-      <c r="B10" s="31"/>
+    <row r="10" spans="1:7" ht="16.399999999999999">
+      <c r="A10" s="33"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="9" t="s">
         <v>26</v>
       </c>
@@ -1430,9 +1501,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16.399999999999999">
-      <c r="A11" s="28"/>
-      <c r="B11" s="31"/>
+    <row r="11" spans="1:7" ht="16.399999999999999">
+      <c r="A11" s="33"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="8" t="s">
         <v>24</v>
       </c>
@@ -1449,9 +1520,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16.399999999999999">
-      <c r="A12" s="29"/>
-      <c r="B12" s="31"/>
+    <row r="12" spans="1:7" ht="16.399999999999999">
+      <c r="A12" s="34"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1468,20 +1539,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-    </row>
-    <row r="14" spans="1:10" ht="16.399999999999999">
-      <c r="A14" s="39" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.399999999999999">
+      <c r="A14" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1500,290 +1571,329 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16.399999999999999">
-      <c r="A15" s="28"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="9" t="s">
+    <row r="15" spans="1:7" ht="16.399999999999999">
+      <c r="A15" s="33"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.399999999999999">
+      <c r="A16" s="33"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D16" s="5">
         <v>812</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="16.399999999999999">
-      <c r="A16" s="28"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="16" t="s">
+      <c r="F16" s="23"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" ht="16.399999999999999">
+      <c r="A17" s="33"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F17" s="22" t="s">
         <v>59</v>
-      </c>
-      <c r="G16" s="2">
-        <v>12</v>
-      </c>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.399999999999999">
-      <c r="A17" s="28"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="5">
-        <v>822</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="G17" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="16.399999999999999">
-      <c r="A18" s="29"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-    </row>
-    <row r="20" spans="1:7" ht="16.399999999999999">
-      <c r="A20" s="40" t="s">
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:10" ht="16.399999999999999">
+      <c r="A18" s="33"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5">
+        <v>822</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16.399999999999999">
+      <c r="A19" s="34"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:10" ht="16.399999999999999">
+      <c r="A21" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B21" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G21" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.399999999999999">
-      <c r="A21" s="41"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="9" t="s">
+    <row r="22" spans="1:10" ht="16.399999999999999">
+      <c r="A22" s="38"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D22" s="5">
         <v>812</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="16.399999999999999">
-      <c r="A22" s="41"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="16" t="s">
+      <c r="E22" s="4"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" ht="16.399999999999999">
+      <c r="A23" s="38"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F23" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G23" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.399999999999999">
-      <c r="A23" s="41"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="6" t="s">
+    <row r="24" spans="1:10" ht="16.399999999999999">
+      <c r="A24" s="38"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D24" s="5">
         <v>822</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F24" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="42"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-    </row>
-    <row r="25" spans="1:7" ht="16.399999999999999">
-      <c r="A25" s="32"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-    </row>
-    <row r="26" spans="1:7" ht="16.399999999999999">
-      <c r="A26" s="34" t="s">
+    <row r="25" spans="1:10">
+      <c r="A25" s="39"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26" spans="1:10" ht="16.399999999999999">
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+    </row>
+    <row r="27" spans="1:10" ht="16.399999999999999">
+      <c r="A27" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B27" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F27" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G27" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16.399999999999999">
-      <c r="A27" s="35"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="9" t="s">
+    <row r="28" spans="1:10" ht="16.399999999999999">
+      <c r="A28" s="27"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="46">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="16.399999999999999">
+      <c r="A29" s="27"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D29" s="5">
         <v>812</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" ht="16.399999999999999">
-      <c r="A28" s="35"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="16" t="s">
+      <c r="E29" s="4"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" ht="16.399999999999999">
+      <c r="A30" s="27"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F30" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G30" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16.399999999999999">
-      <c r="A29" s="35"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="6" t="s">
+    <row r="31" spans="1:10" ht="16.399999999999999">
+      <c r="A31" s="27"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D31" s="5">
         <v>822</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E31" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F31" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G31" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="36"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
+    <row r="32" spans="1:10">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="B6:B12"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1793,16 +1903,17 @@
     <hyperlink ref="C10" r:id="rId4" display="台新銀行"/>
     <hyperlink ref="C8" r:id="rId5" display="國泰世華"/>
     <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="C17" r:id="rId7"/>
-    <hyperlink ref="C23" r:id="rId8"/>
-    <hyperlink ref="C29" r:id="rId9"/>
-    <hyperlink ref="C15" r:id="rId10" display="台新銀行"/>
-    <hyperlink ref="C21" r:id="rId11" display="台新銀行"/>
-    <hyperlink ref="C27" r:id="rId12" display="台新銀行"/>
+    <hyperlink ref="C18" r:id="rId7"/>
+    <hyperlink ref="C24" r:id="rId8"/>
+    <hyperlink ref="C31" r:id="rId9"/>
+    <hyperlink ref="C16" r:id="rId10" display="台新銀行"/>
+    <hyperlink ref="C22" r:id="rId11" display="台新銀行"/>
+    <hyperlink ref="C29" r:id="rId12" display="台新銀行"/>
+    <hyperlink ref="C28" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId14"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
W132 H1900 - Account, Account (lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\共用\Github\Family\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="419" yWindow="105" windowWidth="16979" windowHeight="6336"/>
+    <workbookView xWindow="420" yWindow="110" windowWidth="16980" windowHeight="6340"/>
   </bookViews>
   <sheets>
     <sheet name="金融簡易版" sheetId="4" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <author>Bali-ThinkPad</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +223,42 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0">
+    <comment ref="C24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t xml:space="preserve">網路只可設定非約定
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,17 +298,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>八里龍形</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>700</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -325,14 +361,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>2441268-0053701</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">406-53-4446608       </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>a128509436</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -616,67 +644,189 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>敦南(0023)</t>
+    <t>2888-10-0785170-3</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾辰哲</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2888-10-0786338-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敦南</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0163-979-125049</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>永豐銀行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>807</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北投</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110-018-0012788-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中信綜存</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>天母元大</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">406-51-1527809         </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>822</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>807</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>807</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>110-008-0012788-1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>台新綜存</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>812</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>石牌</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2086-10-0014894-8</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>天母元大</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>700</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2441268-0053701</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>北投</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110-018-0012788-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>永豐外幣</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>北投</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0864-979-166846</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>玉山外幣</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>北投</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0864-879-118113</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>812</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>石牌</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">406-53-4446608       </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>406-51-2020101</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2086-10-0014893-7</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>中華郵政</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>玉山綜存</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>2888-10-0785134-0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2888-10-0785170-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>曾辰哲</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2888-10-0786338-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>敦南</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>玉山綜存</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>808</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>0163-979-125049</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>W312 H0830</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>永豐銀行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>807</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>北投</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110-018-0012788-3</t>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中國信託</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>406-51-2020208</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>W312 H1900</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -783,7 +933,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -894,19 +1044,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -918,7 +1055,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -946,60 +1083,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1008,16 +1104,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1080,7 +1207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1112,9 +1239,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1146,6 +1274,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1321,579 +1450,697 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:J35"/>
+  <dimension ref="A2:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15:F16"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.05" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.25" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="16.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.26953125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="16.399999999999999">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" ht="16.399999999999999">
-      <c r="A3" s="40" t="s">
-        <v>51</v>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.399999999999999">
-      <c r="A4" s="40"/>
+      <c r="C3" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.35">
+      <c r="A4" s="25"/>
       <c r="B4" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="42"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-    </row>
-    <row r="6" spans="1:7" ht="16.399999999999999">
-      <c r="A6" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A6" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G6" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.399999999999999">
-      <c r="A7" s="33"/>
-      <c r="B7" s="36"/>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A7" s="30"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.399999999999999">
-      <c r="A8" s="33"/>
-      <c r="B8" s="36"/>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A8" s="30"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G8" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.399999999999999">
-      <c r="A9" s="33"/>
-      <c r="B9" s="36"/>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A9" s="30"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.399999999999999">
-      <c r="A10" s="33"/>
-      <c r="B10" s="36"/>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A10" s="30"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5">
         <v>812</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.399999999999999">
-      <c r="A11" s="33"/>
-      <c r="B11" s="36"/>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A11" s="30"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" s="5">
         <v>812</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G11" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16.399999999999999">
-      <c r="A12" s="34"/>
-      <c r="B12" s="36"/>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A12" s="31"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="5">
         <v>822</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G12" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-    </row>
-    <row r="14" spans="1:7" ht="16.399999999999999">
-      <c r="A14" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>17</v>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A14" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>14</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G14" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16.399999999999999">
-      <c r="A15" s="33"/>
-      <c r="B15" s="36"/>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A15" s="30"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>60</v>
       </c>
       <c r="G15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.399999999999999">
-      <c r="A16" s="33"/>
-      <c r="B16" s="36"/>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A16" s="30"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5">
         <v>812</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="23"/>
+        <v>20</v>
+      </c>
+      <c r="F16" s="20"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="16.399999999999999">
-      <c r="A17" s="33"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="16" t="s">
-        <v>53</v>
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A17" s="30"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>59</v>
       </c>
       <c r="G17" s="2">
         <v>12</v>
       </c>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" ht="16.399999999999999">
-      <c r="A18" s="33"/>
-      <c r="B18" s="36"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A18" s="30"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="5">
         <v>822</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G18" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16.399999999999999">
-      <c r="A19" s="34"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-    </row>
-    <row r="21" spans="1:10" ht="16.399999999999999">
-      <c r="A21" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>11</v>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A19" s="31"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A21" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>8</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="F21" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="24">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16.399999999999999">
-      <c r="A22" s="38"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="5">
-        <v>812</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" ht="16.399999999999999">
-      <c r="A23" s="38"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="16" t="s">
-        <v>53</v>
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A22" s="40"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A23" s="40"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="43" t="s">
+        <v>77</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>56</v>
+        <v>66</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="G23" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="16.399999999999999">
-      <c r="A24" s="38"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="5">
-        <v>822</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>10</v>
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A24" s="40"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="G24" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="39"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-    </row>
-    <row r="26" spans="1:10" ht="16.399999999999999">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-    </row>
-    <row r="27" spans="1:10" ht="16.399999999999999">
-      <c r="A27" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A25" s="40"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="24">
+        <v>808</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A26" s="40"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A27" s="40"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="G27" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="16.399999999999999">
-      <c r="A28" s="27"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="45" t="s">
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A28" s="40"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="46">
+      <c r="D28" s="22">
+        <v>822</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A29" s="40"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="22">
+        <v>822</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.35">
+      <c r="A30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+    </row>
+    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A31" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.4">
+      <c r="A32" s="25"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="24">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="16.399999999999999">
-      <c r="A29" s="27"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="5">
-        <v>812</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" ht="16.399999999999999">
-      <c r="A30" s="27"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="4" t="s">
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A33" s="25"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A34" s="25"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G30" s="2">
+      <c r="F34" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="16.399999999999999">
-      <c r="A31" s="27"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="5">
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A35" s="25"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="22">
         <v>822</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="15" t="s">
+      <c r="E35" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="2">
+      <c r="F35" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.4">
+      <c r="A36" s="25"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="22">
+        <v>822</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="G36" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="B21:B29"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:A12"/>
     <mergeCell ref="B6:B12"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1904,16 +2151,18 @@
     <hyperlink ref="C8" r:id="rId5" display="國泰世華"/>
     <hyperlink ref="C9" r:id="rId6"/>
     <hyperlink ref="C18" r:id="rId7"/>
-    <hyperlink ref="C24" r:id="rId8"/>
-    <hyperlink ref="C31" r:id="rId9"/>
-    <hyperlink ref="C16" r:id="rId10" display="台新銀行"/>
-    <hyperlink ref="C22" r:id="rId11" display="台新銀行"/>
-    <hyperlink ref="C29" r:id="rId12" display="台新銀行"/>
-    <hyperlink ref="C28" r:id="rId13"/>
+    <hyperlink ref="C16" r:id="rId8" display="台新銀行"/>
+    <hyperlink ref="C19" r:id="rId9" display="中國信託"/>
+    <hyperlink ref="C28" r:id="rId10"/>
+    <hyperlink ref="C29" r:id="rId11"/>
+    <hyperlink ref="C24" r:id="rId12"/>
+    <hyperlink ref="C35" r:id="rId13"/>
+    <hyperlink ref="C36" r:id="rId14"/>
+    <hyperlink ref="C32" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId16"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId15"/>
+  <legacyDrawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
W313 H1600 - All
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\共用\Github\Family\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="110" windowWidth="16980" windowHeight="6340"/>
+    <workbookView xWindow="419" yWindow="105" windowWidth="16979" windowHeight="6336"/>
   </bookViews>
   <sheets>
     <sheet name="金融簡易版" sheetId="4" r:id="rId1"/>
@@ -24,7 +19,7 @@
     <author>Bali-ThinkPad</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0">
+    <comment ref="F11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -189,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
+    <comment ref="C12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C24" authorId="0" shapeId="0">
+    <comment ref="C18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,12 +248,11 @@
             <family val="3"/>
             <charset val="136"/>
           </rPr>
-          <t xml:space="preserve">網路只可設定非約定
-</t>
+          <t>網路只可設定非約定</t>
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0" shapeId="0">
+    <comment ref="C24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -290,6 +284,109 @@
           </rPr>
           <t xml:space="preserve">網路只可設定非約定
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t xml:space="preserve">網路只可設定非約定
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
         </r>
       </text>
     </comment>
@@ -298,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -329,20 +426,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color indexed="12"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>中國信託</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>a128509445</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -680,10 +763,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>中信綜存</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>天母元大</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -800,33 +879,73 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color indexed="12"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-      </rPr>
-      <t>中國信託</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>406-51-2020208</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>W312 H1900</t>
+    <t>台銀</t>
+  </si>
+  <si>
+    <t>台北富邦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>國泰世華</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玉山</t>
+  </si>
+  <si>
+    <t>台新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Richar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>台新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Richar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陳美雲(網路轉帳銀行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中信元大</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾辰哲(網路轉帳銀行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾辰宇(網路轉帳銀行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾正華(網路轉帳銀行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W313 H1600</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -925,15 +1044,21 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1044,6 +1169,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1055,7 +1206,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1097,54 +1248,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1207,7 +1384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1239,10 +1416,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1274,7 +1450,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1450,172 +1625,311 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:J39"/>
+  <dimension ref="A2:AM39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.05" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="16.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.90625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.26953125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.90625" style="1"/>
+    <col min="2" max="2" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="15" width="10.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="5.625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="23" width="10.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="5.625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="10.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="31" width="10.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="5.625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="10.625" style="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="39" width="8.875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="16.399999999999999">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
-        <v>48</v>
+    <row r="3" spans="1:39" ht="16.399999999999999">
+      <c r="A3" s="31" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
+      <c r="C3" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="I3" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="51"/>
+      <c r="Y3" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="54"/>
+      <c r="AF3" s="51"/>
+      <c r="AG3" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH3" s="53"/>
+      <c r="AI3" s="53"/>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="53"/>
+      <c r="AL3" s="53"/>
+      <c r="AM3" s="54"/>
+    </row>
+    <row r="4" spans="1:39" ht="16.399999999999999">
+      <c r="A4" s="31"/>
       <c r="B4" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="I4" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T4" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB4" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ4" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="1:39" ht="16.399999999999999">
+      <c r="A6" s="35" t="s">
         <v>39</v>
       </c>
+      <c r="B6" s="38" t="s">
+        <v>38</v>
+      </c>
       <c r="C6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A7" s="30"/>
-      <c r="B7" s="33"/>
+    <row r="7" spans="1:39" ht="16.399999999999999">
+      <c r="A7" s="36"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A8" s="30"/>
-      <c r="B8" s="33"/>
+    <row r="8" spans="1:39" ht="16.399999999999999">
+      <c r="A8" s="36"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A9" s="30"/>
-      <c r="B9" s="33"/>
+    <row r="9" spans="1:39" ht="16.399999999999999">
+      <c r="A9" s="36"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A10" s="30"/>
-      <c r="B10" s="33"/>
+    <row r="10" spans="1:39" ht="16.399999999999999">
+      <c r="A10" s="36"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5">
         <v>812</v>
@@ -1624,141 +1938,161 @@
         <v>4</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A11" s="30"/>
-      <c r="B11" s="33"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="48"/>
+    </row>
+    <row r="11" spans="1:39" ht="16.399999999999999">
+      <c r="A11" s="36"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="5">
         <v>812</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A12" s="31"/>
-      <c r="B12" s="33"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="O11" s="48"/>
+    </row>
+    <row r="12" spans="1:39" ht="16.399999999999999">
+      <c r="A12" s="37"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="5">
         <v>822</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-    </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A14" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="32" t="s">
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="R12" s="48"/>
+    </row>
+    <row r="13" spans="1:39">
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="1:39" ht="16.399999999999999">
+      <c r="A14" s="44" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="38" t="s">
+        <v>13</v>
+      </c>
       <c r="C14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A15" s="30"/>
-      <c r="B15" s="33"/>
+    <row r="15" spans="1:39" ht="16.399999999999999">
+      <c r="A15" s="36"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="20" t="s">
         <v>59</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>60</v>
       </c>
       <c r="G15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A16" s="30"/>
-      <c r="B16" s="33"/>
+    <row r="16" spans="1:39" ht="16.399999999999999">
+      <c r="A16" s="36"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="5">
         <v>812</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A17" s="30"/>
-      <c r="B17" s="33"/>
+    <row r="17" spans="1:14" ht="16.399999999999999">
+      <c r="A17" s="36"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="2">
         <v>12</v>
       </c>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A18" s="30"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="6" t="s">
-        <v>5</v>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+    </row>
+    <row r="18" spans="1:14" ht="16.399999999999999">
+      <c r="A18" s="36"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="D18" s="5">
         <v>822</v>
@@ -1767,182 +2101,182 @@
         <v>4</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A19" s="31"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="8" t="s">
+    <row r="19" spans="1:14" ht="16.399999999999999">
+      <c r="A19" s="37"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="23" t="s">
         <v>61</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>63</v>
       </c>
       <c r="G19" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-    </row>
-    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A21" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>8</v>
+    <row r="20" spans="1:14">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="1:14" ht="16.399999999999999" customHeight="1">
+      <c r="A21" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>7</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="26" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G21" s="24">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A22" s="40"/>
-      <c r="B22" s="36"/>
+    <row r="22" spans="1:14" ht="16.399999999999999" customHeight="1">
+      <c r="A22" s="46"/>
+      <c r="B22" s="42"/>
       <c r="C22" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G22" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A23" s="40"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="43" t="s">
-        <v>77</v>
+    <row r="23" spans="1:14" ht="16.399999999999999" customHeight="1">
+      <c r="A23" s="46"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G23" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A24" s="40"/>
-      <c r="B24" s="36"/>
+    <row r="24" spans="1:14" ht="16.399999999999999" customHeight="1">
+      <c r="A24" s="46"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>78</v>
+        <v>25</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>76</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G24" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A25" s="40"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="44" t="s">
-        <v>80</v>
+    <row r="25" spans="1:14" ht="16.399999999999999" customHeight="1">
+      <c r="A25" s="46"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="28" t="s">
+        <v>78</v>
       </c>
       <c r="D25" s="24">
         <v>808</v>
       </c>
-      <c r="E25" s="42" t="s">
-        <v>81</v>
+      <c r="E25" s="26" t="s">
+        <v>79</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G25" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A26" s="40"/>
-      <c r="B26" s="36"/>
+    <row r="26" spans="1:14" ht="16.399999999999999">
+      <c r="A26" s="46"/>
+      <c r="B26" s="42"/>
       <c r="C26" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>82</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G26" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A27" s="40"/>
-      <c r="B27" s="36"/>
+    <row r="27" spans="1:14" ht="16.399999999999999">
+      <c r="A27" s="46"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>51</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>52</v>
       </c>
       <c r="G27" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A28" s="40"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="6" t="s">
-        <v>5</v>
+    <row r="28" spans="1:14" ht="16.399999999999999">
+      <c r="A28" s="46"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="D28" s="22">
         <v>822</v>
@@ -1951,54 +2285,54 @@
         <v>4</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G28" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A29" s="40"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="6" t="s">
-        <v>5</v>
+    <row r="29" spans="1:14" ht="16.399999999999999" customHeight="1">
+      <c r="A29" s="47"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="D29" s="22">
         <v>822</v>
       </c>
-      <c r="E29" s="41" t="s">
-        <v>72</v>
+      <c r="E29" s="25" t="s">
+        <v>70</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G29" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.35">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-    </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A31" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="36" t="s">
+    <row r="30" spans="1:14" ht="16.399999999999999">
+      <c r="A30" s="40"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+    </row>
+    <row r="31" spans="1:14" ht="16.399999999999999">
+      <c r="A31" s="31" t="s">
         <v>6</v>
       </c>
+      <c r="B31" s="42" t="s">
+        <v>5</v>
+      </c>
       <c r="C31" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="26" t="s">
         <v>1</v>
       </c>
       <c r="F31" s="23" t="s">
@@ -2008,68 +2342,68 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.4">
-      <c r="A32" s="25"/>
-      <c r="B32" s="36"/>
+    <row r="32" spans="1:14" ht="16.399999999999999">
+      <c r="A32" s="31"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E32" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G32" s="24">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A33" s="25"/>
-      <c r="B33" s="36"/>
+    <row r="33" spans="1:7" ht="16.399999999999999">
+      <c r="A33" s="31"/>
+      <c r="B33" s="42"/>
       <c r="C33" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>70</v>
-      </c>
       <c r="F33" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G33" s="24">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A34" s="25"/>
-      <c r="B34" s="36"/>
+    <row r="34" spans="1:7" ht="16.399999999999999">
+      <c r="A34" s="31"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E34" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G34" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A35" s="25"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="6" t="s">
-        <v>91</v>
+    <row r="35" spans="1:7" ht="16.399999999999999">
+      <c r="A35" s="31"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="D35" s="22">
         <v>822</v>
@@ -2084,26 +2418,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.4">
-      <c r="A36" s="25"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="6" t="s">
-        <v>91</v>
+    <row r="36" spans="1:7" ht="16.399999999999999">
+      <c r="A36" s="31"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="D36" s="22">
         <v>822</v>
       </c>
-      <c r="E36" s="41" t="s">
-        <v>72</v>
+      <c r="E36" s="25" t="s">
+        <v>70</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G36" s="24">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="17"/>
@@ -2112,7 +2446,7 @@
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
@@ -2121,12 +2455,16 @@
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="18">
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="Y3:AE3"/>
+    <mergeCell ref="AG3:AM3"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="B31:B36"/>
@@ -2150,15 +2488,15 @@
     <hyperlink ref="C10" r:id="rId4" display="台新銀行"/>
     <hyperlink ref="C8" r:id="rId5" display="國泰世華"/>
     <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="C18" r:id="rId7"/>
-    <hyperlink ref="C16" r:id="rId8" display="台新銀行"/>
-    <hyperlink ref="C19" r:id="rId9" display="中國信託"/>
-    <hyperlink ref="C28" r:id="rId10"/>
-    <hyperlink ref="C29" r:id="rId11"/>
-    <hyperlink ref="C24" r:id="rId12"/>
-    <hyperlink ref="C35" r:id="rId13"/>
-    <hyperlink ref="C36" r:id="rId14"/>
-    <hyperlink ref="C32" r:id="rId15"/>
+    <hyperlink ref="C16" r:id="rId7" display="台新銀行"/>
+    <hyperlink ref="C24" r:id="rId8"/>
+    <hyperlink ref="C36" r:id="rId9" display="中國信託"/>
+    <hyperlink ref="C32" r:id="rId10"/>
+    <hyperlink ref="C18" r:id="rId11" display="中國信託"/>
+    <hyperlink ref="C28" r:id="rId12" display="中國信託"/>
+    <hyperlink ref="C35" r:id="rId13" display="中國信託"/>
+    <hyperlink ref="C19" r:id="rId14" display="中國信託"/>
+    <hyperlink ref="C29" r:id="rId15" display="中國信託"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId16"/>

</xml_diff>

<commit_message>
W314 H1530 - Account (lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="107">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -937,7 +937,40 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W313 H1600</t>
+    <t>個人設定/常用帳戶設定/約定帳號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>台幣轉帳</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>轉入帳號設定</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W314 H1530</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1206,7 +1239,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1258,53 +1291,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1321,6 +1307,56 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1647,19 +1683,19 @@
     <col min="5" max="5" width="13.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="26.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="15" width="10.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="27" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" style="1" customWidth="1"/>
+    <col min="10" max="15" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
     <col min="16" max="16" width="5.625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="23" width="10.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="10.625" style="1" customWidth="1"/>
+    <col min="18" max="23" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
     <col min="24" max="24" width="5.625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="10.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="31" width="10.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="10.625" style="1" customWidth="1"/>
+    <col min="26" max="31" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
     <col min="32" max="32" width="5.625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="10.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="10.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="39" width="8.875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="10.625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="39" width="8.875" style="1" customWidth="1" outlineLevel="1"/>
     <col min="40" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
@@ -1670,66 +1706,66 @@
         <v>48</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:39" ht="16.399999999999999">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="40" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="I3" s="52" t="s">
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="I3" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="54"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="37"/>
       <c r="P3" s="29"/>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="52" t="s">
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="36"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53"/>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="52" t="s">
+      <c r="Z3" s="36"/>
+      <c r="AA3" s="36"/>
+      <c r="AB3" s="36"/>
+      <c r="AC3" s="36"/>
+      <c r="AD3" s="36"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="34"/>
+      <c r="AG3" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="54"/>
+      <c r="AH3" s="36"/>
+      <c r="AI3" s="36"/>
+      <c r="AJ3" s="36"/>
+      <c r="AK3" s="36"/>
+      <c r="AL3" s="36"/>
+      <c r="AM3" s="37"/>
     </row>
     <row r="4" spans="1:39" ht="16.399999999999999">
-      <c r="A4" s="31"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
@@ -1748,7 +1784,7 @@
       <c r="G4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="50" t="s">
+      <c r="I4" s="33" t="s">
         <v>90</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1757,7 +1793,7 @@
       <c r="K4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="50" t="s">
+      <c r="L4" s="33" t="s">
         <v>93</v>
       </c>
       <c r="M4" s="2" t="s">
@@ -1770,7 +1806,7 @@
         <v>95</v>
       </c>
       <c r="P4" s="29"/>
-      <c r="Q4" s="50" t="s">
+      <c r="Q4" s="33" t="s">
         <v>90</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -1779,7 +1815,7 @@
       <c r="S4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="T4" s="50" t="s">
+      <c r="T4" s="33" t="s">
         <v>93</v>
       </c>
       <c r="U4" s="2" t="s">
@@ -1792,7 +1828,7 @@
         <v>95</v>
       </c>
       <c r="X4" s="30"/>
-      <c r="Y4" s="50" t="s">
+      <c r="Y4" s="33" t="s">
         <v>90</v>
       </c>
       <c r="Z4" s="2" t="s">
@@ -1801,7 +1837,7 @@
       <c r="AA4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AB4" s="50" t="s">
+      <c r="AB4" s="33" t="s">
         <v>93</v>
       </c>
       <c r="AC4" s="2" t="s">
@@ -1814,7 +1850,7 @@
         <v>95</v>
       </c>
       <c r="AF4" s="30"/>
-      <c r="AG4" s="50" t="s">
+      <c r="AG4" s="33" t="s">
         <v>90</v>
       </c>
       <c r="AH4" s="2" t="s">
@@ -1823,7 +1859,7 @@
       <c r="AI4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AJ4" s="50" t="s">
+      <c r="AJ4" s="33" t="s">
         <v>93</v>
       </c>
       <c r="AK4" s="2" t="s">
@@ -1837,19 +1873,19 @@
       </c>
     </row>
     <row r="5" spans="1:39">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="1:39" ht="16.399999999999999">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="47" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1869,8 +1905,8 @@
       </c>
     </row>
     <row r="7" spans="1:39" ht="16.399999999999999">
-      <c r="A7" s="36"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="48"/>
       <c r="C7" s="9" t="s">
         <v>33</v>
       </c>
@@ -1886,10 +1922,13 @@
       <c r="G7" s="2">
         <v>13</v>
       </c>
+      <c r="H7" s="55" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="8" spans="1:39" ht="16.399999999999999">
-      <c r="A8" s="36"/>
-      <c r="B8" s="39"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="48"/>
       <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
@@ -1907,8 +1946,8 @@
       </c>
     </row>
     <row r="9" spans="1:39" ht="16.399999999999999">
-      <c r="A9" s="36"/>
-      <c r="B9" s="39"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="8" t="s">
         <v>26</v>
       </c>
@@ -1926,8 +1965,8 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="16.399999999999999">
-      <c r="A10" s="36"/>
-      <c r="B10" s="39"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
@@ -1943,16 +1982,16 @@
       <c r="G10" s="2">
         <v>14</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="48"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="31"/>
     </row>
     <row r="11" spans="1:39" ht="16.399999999999999">
-      <c r="A11" s="36"/>
-      <c r="B11" s="39"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
@@ -1968,16 +2007,16 @@
       <c r="G11" s="2">
         <v>14</v>
       </c>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="O11" s="48"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="O11" s="31"/>
     </row>
     <row r="12" spans="1:39" ht="16.399999999999999">
-      <c r="A12" s="37"/>
-      <c r="B12" s="39"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1993,28 +2032,41 @@
       <c r="G12" s="2">
         <v>12</v>
       </c>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="R12" s="48"/>
+      <c r="H12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="AB12" s="31"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31"/>
+      <c r="AJ12" s="31"/>
+      <c r="AK12" s="31"/>
+      <c r="AL12" s="31"/>
+      <c r="AM12" s="31"/>
     </row>
     <row r="13" spans="1:39">
-      <c r="A13" s="43"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
     </row>
     <row r="14" spans="1:39" ht="16.399999999999999">
       <c r="A14" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="47" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -2034,8 +2086,8 @@
       </c>
     </row>
     <row r="15" spans="1:39" ht="16.399999999999999">
-      <c r="A15" s="36"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="6" t="s">
         <v>56</v>
       </c>
@@ -2053,8 +2105,8 @@
       </c>
     </row>
     <row r="16" spans="1:39" ht="16.399999999999999">
-      <c r="A16" s="36"/>
-      <c r="B16" s="39"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="9" t="s">
         <v>22</v>
       </c>
@@ -2068,8 +2120,8 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:14" ht="16.399999999999999">
-      <c r="A17" s="36"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="15" t="s">
         <v>49</v>
       </c>
@@ -2089,8 +2141,8 @@
       <c r="N17" s="18"/>
     </row>
     <row r="18" spans="1:14" ht="16.399999999999999">
-      <c r="A18" s="36"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="8" t="s">
         <v>17</v>
       </c>
@@ -2108,8 +2160,8 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="16.399999999999999">
-      <c r="A19" s="37"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="9" t="s">
         <v>100</v>
       </c>
@@ -2127,19 +2179,19 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
     </row>
     <row r="21" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -2159,8 +2211,8 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="42"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="15" t="s">
         <v>56</v>
       </c>
@@ -2178,8 +2230,8 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A23" s="46"/>
-      <c r="B23" s="42"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="27" t="s">
         <v>75</v>
       </c>
@@ -2197,8 +2249,8 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A24" s="46"/>
-      <c r="B24" s="42"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="8" t="s">
         <v>26</v>
       </c>
@@ -2216,8 +2268,8 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A25" s="46"/>
-      <c r="B25" s="42"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="28" t="s">
         <v>78</v>
       </c>
@@ -2235,8 +2287,8 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="16.399999999999999">
-      <c r="A26" s="46"/>
-      <c r="B26" s="42"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="8" t="s">
         <v>66</v>
       </c>
@@ -2254,8 +2306,8 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="16.399999999999999">
-      <c r="A27" s="46"/>
-      <c r="B27" s="42"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="15" t="s">
         <v>49</v>
       </c>
@@ -2273,8 +2325,8 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="16.399999999999999">
-      <c r="A28" s="46"/>
-      <c r="B28" s="42"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="8" t="s">
         <v>17</v>
       </c>
@@ -2292,8 +2344,8 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A29" s="47"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="51"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="9" t="s">
         <v>100</v>
       </c>
@@ -2311,19 +2363,19 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="16.399999999999999">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:14" ht="16.399999999999999">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -2343,8 +2395,8 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="16.399999999999999">
-      <c r="A32" s="31"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="8" t="s">
         <v>87</v>
       </c>
@@ -2362,8 +2414,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="16.399999999999999">
-      <c r="A33" s="31"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="8" t="s">
         <v>66</v>
       </c>
@@ -2381,8 +2433,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="16.399999999999999">
-      <c r="A34" s="31"/>
-      <c r="B34" s="42"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="15" t="s">
         <v>49</v>
       </c>
@@ -2400,8 +2452,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="16.399999999999999">
-      <c r="A35" s="31"/>
-      <c r="B35" s="42"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="8" t="s">
         <v>17</v>
       </c>
@@ -2419,8 +2471,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="16.399999999999999">
-      <c r="A36" s="31"/>
-      <c r="B36" s="42"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="9" t="s">
         <v>100</v>
       </c>
@@ -2461,11 +2513,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="Y3:AE3"/>
-    <mergeCell ref="AG3:AM3"/>
-    <mergeCell ref="A30:G30"/>
     <mergeCell ref="A31:A36"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="A13:G13"/>
@@ -2474,6 +2521,11 @@
     <mergeCell ref="A20:G20"/>
     <mergeCell ref="A21:A29"/>
     <mergeCell ref="B21:B29"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="Y3:AE3"/>
+    <mergeCell ref="AG3:AM3"/>
+    <mergeCell ref="A30:G30"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A5:G5"/>

</xml_diff>

<commit_message>
W315 H1400 - Account (lite), Currency
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="金融簡易版" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -69,15 +70,14 @@
         </r>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="細明體"/>
             <family val="3"/>
             <charset val="136"/>
           </rPr>
-          <t xml:space="preserve">網路可設定約定及非約定
-</t>
+          <t>網路可設定約定及非約定
+需金融卡認證</t>
         </r>
       </text>
     </comment>
@@ -145,8 +145,101 @@
             <family val="3"/>
             <charset val="136"/>
           </rPr>
-          <t xml:space="preserve">網路只可設定非約定
+          <t xml:space="preserve">網路可設定約定及非約定
+需金融卡認證
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>臨櫃申請線上約定帳號設定:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>轉帳</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>線上約定帳號設定</t>
         </r>
       </text>
     </comment>
@@ -214,31 +307,18 @@
             <family val="3"/>
             <charset val="136"/>
           </rPr>
-          <t>網路只可設定非約定</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C18" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bali-ThinkPad:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+          <t>網路只可設定非約定
+別名設定:
+個人設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
         </r>
         <r>
           <rPr>
@@ -248,31 +328,16 @@
             <family val="3"/>
             <charset val="136"/>
           </rPr>
-          <t>網路只可設定非約定</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bali-ThinkPad:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+          <t>常用帳戶設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
         </r>
         <r>
           <rPr>
@@ -282,12 +347,11 @@
             <family val="3"/>
             <charset val="136"/>
           </rPr>
-          <t xml:space="preserve">網路只可設定非約定
-</t>
+          <t>約定帳號</t>
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0">
+    <comment ref="C19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -321,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0">
+    <comment ref="H19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -351,12 +415,621 @@
             <family val="3"/>
             <charset val="136"/>
           </rPr>
+          <t>刪華彰化</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
           <t xml:space="preserve">網路只可設定非約定
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C35" authorId="0">
+    <comment ref="C29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t xml:space="preserve">網路只可設定非約定
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Bali-ThinkPad</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>臨櫃申請線上約定帳號設定:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>轉帳</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>線上約定帳號設定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>臨櫃申請線上約定帳號設定:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>轉帳</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>線上約定帳號設定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>忽略敦南分行碼:0023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>忽略敦南分行碼:0023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定
+別名設定:
+個人設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>常用帳戶設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>約定帳號</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -395,7 +1068,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="117">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -735,10 +1408,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>2888-10-0786338-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>敦南</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -917,60 +1586,77 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>中信元大</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾辰哲(網路轉帳銀行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾辰宇(網路轉帳銀行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾正華(網路轉帳銀行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>陳美雲(網路轉帳銀行)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>永豐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中華郵政</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>永豐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>中信元大</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>曾辰哲(網路轉帳銀行)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>曾辰宇(網路轉帳銀行)</t>
+    <t>2888-10-0786338-8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>曾正華(網路轉帳銀行)</t>
+    <t>台新綜存</t>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>個人設定/常用帳戶設定/約定帳號</t>
+    <t>台新</t>
+  </si>
+  <si>
+    <t>天母元大</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">406-51-1527809         </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾正華</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>台幣轉帳</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="細明體"/>
-        <family val="3"/>
-        <charset val="136"/>
-      </rPr>
-      <t>轉入帳號設定</t>
-    </r>
+    <t>曾辰宇</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W314 H1530</t>
+    <t>曾辰哲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W315 H1400</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -978,7 +1664,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1061,14 +1747,6 @@
       <charset val="136"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="細明體"/>
-      <family val="3"/>
-      <charset val="136"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color indexed="12"/>
@@ -1077,7 +1755,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1087,6 +1765,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1239,7 +1923,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1267,11 +1951,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1283,7 +1966,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1299,20 +1982,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1348,6 +2020,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1355,8 +2042,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1665,7 +2376,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:AM39"/>
+  <dimension ref="A2:AL42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
@@ -1683,89 +2394,88 @@
     <col min="5" max="5" width="13.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="26.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="5.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.625" style="1" customWidth="1"/>
-    <col min="10" max="15" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="5.625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.625" style="1" customWidth="1"/>
-    <col min="18" max="23" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="16" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.625" style="1" customWidth="1"/>
+    <col min="19" max="23" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
     <col min="24" max="24" width="5.625" style="1" customWidth="1"/>
     <col min="25" max="25" width="10.625" style="1" customWidth="1"/>
     <col min="26" max="31" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
     <col min="32" max="32" width="5.625" style="1" customWidth="1"/>
     <col min="33" max="33" width="10.625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="39" width="8.875" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="16384" width="8.875" style="1"/>
+    <col min="34" max="38" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:39" ht="16.399999999999999">
+    <row r="2" spans="1:38" ht="16.399999999999999">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
-    </row>
-    <row r="3" spans="1:39" ht="16.399999999999999">
-      <c r="A3" s="40" t="s">
+      <c r="R2" s="18"/>
+    </row>
+    <row r="3" spans="1:38" ht="16.399999999999999">
+      <c r="A3" s="36" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="I3" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="35" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="I3" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z3" s="36"/>
-      <c r="AA3" s="36"/>
-      <c r="AB3" s="36"/>
-      <c r="AC3" s="36"/>
-      <c r="AD3" s="36"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="34"/>
-      <c r="AG3" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH3" s="36"/>
-      <c r="AI3" s="36"/>
-      <c r="AJ3" s="36"/>
-      <c r="AK3" s="36"/>
-      <c r="AL3" s="36"/>
-      <c r="AM3" s="37"/>
-    </row>
-    <row r="4" spans="1:39" ht="16.399999999999999">
-      <c r="A4" s="40"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="50"/>
+      <c r="AF3" s="33"/>
+      <c r="AG3" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="49"/>
+      <c r="AL3" s="50"/>
+    </row>
+    <row r="4" spans="1:38" ht="16.399999999999999">
+      <c r="A4" s="36"/>
       <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
@@ -1784,108 +2494,105 @@
       <c r="G4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="M4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="S4" s="2" t="s">
+      <c r="V4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA4" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="T4" s="33" t="s">
+      <c r="AB4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="AC4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="V4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="W4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH4" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB4" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ4" s="33" t="s">
-        <v>93</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>94</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-    </row>
-    <row r="6" spans="1:39" ht="16.399999999999999">
-      <c r="A6" s="54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38">
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+    </row>
+    <row r="6" spans="1:38" ht="16.399999999999999">
+      <c r="A6" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="43" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1904,9 +2611,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="16.399999999999999">
-      <c r="A7" s="45"/>
-      <c r="B7" s="48"/>
+    <row r="7" spans="1:38" ht="16.399999999999999">
+      <c r="A7" s="41"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="9" t="s">
         <v>33</v>
       </c>
@@ -1922,13 +2629,11 @@
       <c r="G7" s="2">
         <v>13</v>
       </c>
-      <c r="H7" s="55" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" ht="16.399999999999999">
-      <c r="A8" s="45"/>
-      <c r="B8" s="48"/>
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:38" ht="16.399999999999999">
+      <c r="A8" s="41"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
@@ -1945,9 +2650,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="16.399999999999999">
-      <c r="A9" s="45"/>
-      <c r="B9" s="48"/>
+    <row r="9" spans="1:38" ht="16.399999999999999">
+      <c r="A9" s="41"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="8" t="s">
         <v>26</v>
       </c>
@@ -1964,9 +2669,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="16.399999999999999">
-      <c r="A10" s="45"/>
-      <c r="B10" s="48"/>
+    <row r="10" spans="1:38" ht="16.399999999999999">
+      <c r="A10" s="41"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
@@ -1982,16 +2687,42 @@
       <c r="G10" s="2">
         <v>14</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="31"/>
-    </row>
-    <row r="11" spans="1:39" ht="16.399999999999999">
-      <c r="A11" s="45"/>
-      <c r="B11" s="48"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="T10" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="U10" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="V10" s="30"/>
+      <c r="W10" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB10" s="30"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI10" s="30"/>
+      <c r="AJ10" s="30"/>
+      <c r="AK10" s="30"/>
+      <c r="AL10" s="60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" ht="16.399999999999999">
+      <c r="A11" s="41"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
@@ -2007,552 +2738,1523 @@
       <c r="G11" s="2">
         <v>14</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="O11" s="31"/>
-    </row>
-    <row r="12" spans="1:39" ht="16.399999999999999">
-      <c r="A12" s="46"/>
-      <c r="B12" s="48"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="T11" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="U11" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="V11" s="30"/>
+      <c r="W11" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="30"/>
+      <c r="AE11" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI11" s="30"/>
+      <c r="AJ11" s="30"/>
+      <c r="AK11" s="30"/>
+      <c r="AL11" s="60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="16.399999999999999">
+      <c r="A12" s="41"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="5">
         <v>822</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="34" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="2">
         <v>12</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
       <c r="N12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="31"/>
-      <c r="AB12" s="31"/>
-      <c r="AC12" s="31"/>
-      <c r="AD12" s="31"/>
-      <c r="AE12" s="31"/>
-      <c r="AJ12" s="31"/>
-      <c r="AK12" s="31"/>
-      <c r="AL12" s="31"/>
-      <c r="AM12" s="31"/>
-    </row>
-    <row r="13" spans="1:39">
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="30"/>
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="30"/>
+      <c r="AD12" s="30"/>
+      <c r="AE12" s="30"/>
+      <c r="AH12" s="30"/>
+      <c r="AI12" s="30"/>
+      <c r="AJ12" s="30"/>
+      <c r="AK12" s="30"/>
+      <c r="AL12" s="30"/>
+    </row>
+    <row r="13" spans="1:38" ht="16.399999999999999">
       <c r="A13" s="42"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-    </row>
-    <row r="14" spans="1:39" ht="16.399999999999999">
-      <c r="A14" s="44" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="5">
+        <v>822</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="23">
+        <v>12</v>
+      </c>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="30"/>
+      <c r="AE13" s="30"/>
+      <c r="AH13" s="30"/>
+      <c r="AI13" s="30"/>
+      <c r="AJ13" s="30"/>
+      <c r="AK13" s="30"/>
+      <c r="AL13" s="30"/>
+    </row>
+    <row r="14" spans="1:38">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="P14" s="56"/>
+      <c r="W14" s="56"/>
+      <c r="AE14" s="56"/>
+      <c r="AL14" s="56"/>
+    </row>
+    <row r="15" spans="1:38" ht="16.399999999999999">
+      <c r="A15" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B15" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G15" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:39" ht="16.399999999999999">
-      <c r="A15" s="45"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="6" t="s">
+      <c r="L15" s="30"/>
+      <c r="M15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="N15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="O15" s="30"/>
+      <c r="P15" s="57"/>
+      <c r="S15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="T15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="U15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="V15" s="30"/>
+      <c r="W15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD15" s="30"/>
+      <c r="AE15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ15" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK15" s="30"/>
+      <c r="AL15" s="60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" ht="16.399999999999999">
+      <c r="A16" s="41"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="G16" s="2">
+        <v>14</v>
+      </c>
+      <c r="P16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="AE16" s="56"/>
+      <c r="AL16" s="56"/>
+    </row>
+    <row r="17" spans="1:38" ht="16.399999999999999">
+      <c r="A17" s="41"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="2">
+        <v>14</v>
+      </c>
+      <c r="M17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="N17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="O17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="P17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="R17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="S17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="T17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="U17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="V17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="W17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK17" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL17" s="60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" ht="16.399999999999999">
+      <c r="A18" s="41"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="2">
+        <v>14</v>
+      </c>
+      <c r="M18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="N18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="O18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="P18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="R18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="S18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="T18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="U18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="V18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="W18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK18" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL18" s="60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" ht="16.399999999999999">
+      <c r="A19" s="41"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="5">
+        <v>822</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="2">
+        <v>12</v>
+      </c>
+      <c r="I19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="R19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="S19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="T19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="U19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="AB19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD19" s="30"/>
+      <c r="AE19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ19" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK19" s="30"/>
+      <c r="AL19" s="60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" ht="16.399999999999999">
+      <c r="A20" s="42"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="2">
+      <c r="F20" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="23">
+        <v>12</v>
+      </c>
+      <c r="I20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="R20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="S20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="T20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="U20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="AB20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD20" s="30"/>
+      <c r="AE20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ20" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK20" s="30"/>
+      <c r="AL20" s="60" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38">
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="P21" s="56"/>
+      <c r="W21" s="56"/>
+      <c r="AE21" s="56"/>
+      <c r="AL21" s="56"/>
+    </row>
+    <row r="22" spans="1:38" ht="16.399999999999999" customHeight="1">
+      <c r="A22" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="23">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" ht="16.399999999999999">
-      <c r="A16" s="45"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="5">
-        <v>812</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:14" ht="16.399999999999999">
-      <c r="A17" s="45"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="2">
-        <v>12</v>
-      </c>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-    </row>
-    <row r="18" spans="1:14" ht="16.399999999999999">
-      <c r="A18" s="45"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="5">
-        <v>822</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="16.399999999999999">
-      <c r="A19" s="46"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="22" t="s">
+      <c r="P22" s="56"/>
+      <c r="W22" s="56"/>
+      <c r="AL22" s="56"/>
+    </row>
+    <row r="23" spans="1:38" ht="16.399999999999999" customHeight="1">
+      <c r="A23" s="46"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-    </row>
-    <row r="21" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A21" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="23" t="s">
+      <c r="E23" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A22" s="50"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="F23" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A23" s="50"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>65</v>
       </c>
       <c r="G23" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A24" s="50"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="8" t="s">
+      <c r="P23" s="56"/>
+      <c r="W23" s="56"/>
+    </row>
+    <row r="24" spans="1:38" ht="16.399999999999999" customHeight="1">
+      <c r="A24" s="46"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="2">
+        <v>14</v>
+      </c>
+      <c r="P24" s="56"/>
+      <c r="W24" s="56"/>
+    </row>
+    <row r="25" spans="1:38" ht="16.399999999999999" customHeight="1">
+      <c r="A25" s="46"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D25" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E25" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A25" s="50"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="24">
-        <v>808</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>80</v>
       </c>
       <c r="G25" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="16.399999999999999">
-      <c r="A26" s="50"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="22" t="s">
+      <c r="P25" s="56"/>
+      <c r="W25" s="56"/>
+    </row>
+    <row r="26" spans="1:38" ht="16.399999999999999" customHeight="1">
+      <c r="A26" s="46"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="23">
+        <v>808</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="2">
+        <v>13</v>
+      </c>
+      <c r="P26" s="56"/>
+    </row>
+    <row r="27" spans="1:38" ht="16.399999999999999">
+      <c r="A27" s="46"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="16.399999999999999">
-      <c r="A27" s="50"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>51</v>
+      <c r="F27" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="G27" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="16.399999999999999">
-      <c r="A28" s="50"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="8" t="s">
+      <c r="P27" s="56"/>
+    </row>
+    <row r="28" spans="1:38" ht="16.399999999999999">
+      <c r="A28" s="46"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="2">
+        <v>14</v>
+      </c>
+      <c r="P28" s="56"/>
+    </row>
+    <row r="29" spans="1:38" ht="16.399999999999999">
+      <c r="A29" s="46"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D29" s="21">
         <v>822</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E29" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F29" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="23">
+        <v>12</v>
+      </c>
+      <c r="P29" s="56"/>
+    </row>
+    <row r="30" spans="1:38" ht="16.399999999999999" customHeight="1">
+      <c r="A30" s="47"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="21">
+        <v>822</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G30" s="23">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="16.399999999999999" customHeight="1">
-      <c r="A29" s="51"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="22">
+      <c r="P30" s="56"/>
+    </row>
+    <row r="31" spans="1:38" ht="16.399999999999999">
+      <c r="A31" s="51"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="P31" s="56"/>
+    </row>
+    <row r="32" spans="1:38" ht="16.399999999999999">
+      <c r="A32" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="23">
+        <v>14</v>
+      </c>
+      <c r="P32" s="56"/>
+    </row>
+    <row r="33" spans="1:16" ht="16.399999999999999">
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="23">
+        <v>13</v>
+      </c>
+      <c r="P33" s="56"/>
+    </row>
+    <row r="34" spans="1:16" ht="16.399999999999999">
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" s="23">
+        <v>14</v>
+      </c>
+      <c r="P34" s="56"/>
+    </row>
+    <row r="35" spans="1:16" ht="16.399999999999999">
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="2">
+        <v>14</v>
+      </c>
+      <c r="P35" s="56"/>
+    </row>
+    <row r="36" spans="1:16" ht="16.399999999999999">
+      <c r="A36" s="36"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="21">
         <v>822</v>
       </c>
-      <c r="E29" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="24">
+      <c r="E36" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="23">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="16.399999999999999">
-      <c r="A30" s="38"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-    </row>
-    <row r="31" spans="1:14" ht="16.399999999999999">
-      <c r="A31" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="G31" s="24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="16.399999999999999">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="G32" s="24">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="16.399999999999999">
-      <c r="A33" s="40"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G33" s="24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="16.399999999999999">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" s="21" t="s">
+      <c r="P36" s="56"/>
+    </row>
+    <row r="37" spans="1:16" ht="16.399999999999999">
+      <c r="A37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="21">
+        <v>822</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F37" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G34" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="16.399999999999999">
-      <c r="A35" s="40"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="22">
-        <v>822</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35" s="24">
+      <c r="G37" s="23">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="16.399999999999999">
-      <c r="A36" s="40"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D36" s="22">
-        <v>822</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="G36" s="24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
+      <c r="P37" s="56"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="P38" s="56"/>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="P39" s="56"/>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="P40" s="56"/>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="P41" s="56"/>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="P42" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="B21:B29"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="R3:W3"/>
     <mergeCell ref="Y3:AE3"/>
-    <mergeCell ref="AG3:AM3"/>
-    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="AG3:AL3"/>
+    <mergeCell ref="A31:G31"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="A6:A13"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="I3:P3"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" display="中國信託"/>
-    <hyperlink ref="C6" r:id="rId2" display="台灣營行"/>
-    <hyperlink ref="C14" r:id="rId3"/>
-    <hyperlink ref="C10" r:id="rId4" display="台新銀行"/>
-    <hyperlink ref="C8" r:id="rId5" display="國泰世華"/>
-    <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="C16" r:id="rId7" display="台新銀行"/>
-    <hyperlink ref="C24" r:id="rId8"/>
-    <hyperlink ref="C36" r:id="rId9" display="中國信託"/>
-    <hyperlink ref="C32" r:id="rId10"/>
-    <hyperlink ref="C18" r:id="rId11" display="中國信託"/>
-    <hyperlink ref="C28" r:id="rId12" display="中國信託"/>
-    <hyperlink ref="C35" r:id="rId13" display="中國信託"/>
-    <hyperlink ref="C19" r:id="rId14" display="中國信託"/>
-    <hyperlink ref="C29" r:id="rId15" display="中國信託"/>
+    <hyperlink ref="C6" r:id="rId1" display="台灣營行"/>
+    <hyperlink ref="C15" r:id="rId2"/>
+    <hyperlink ref="C10" r:id="rId3" display="台新銀行"/>
+    <hyperlink ref="C8" r:id="rId4" display="國泰世華"/>
+    <hyperlink ref="C9" r:id="rId5"/>
+    <hyperlink ref="C25" r:id="rId6"/>
+    <hyperlink ref="C37" r:id="rId7" display="中國信託"/>
+    <hyperlink ref="C33" r:id="rId8"/>
+    <hyperlink ref="C19" r:id="rId9" display="中國信託"/>
+    <hyperlink ref="C29" r:id="rId10" display="中國信託"/>
+    <hyperlink ref="C36" r:id="rId11" display="中國信託"/>
+    <hyperlink ref="C20" r:id="rId12" display="中國信託"/>
+    <hyperlink ref="C30" r:id="rId13" display="中國信託"/>
+    <hyperlink ref="C12" r:id="rId14" display="中國信託"/>
+    <hyperlink ref="C13" r:id="rId15" display="中國信託"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId16"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId17"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:N22"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.399999999999999"/>
+  <cols>
+    <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="15.25" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="24.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14">
+      <c r="A2" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5">
+        <v>812</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2">
+        <v>14</v>
+      </c>
+      <c r="I2" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="5">
+        <v>812</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="67"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5">
+        <v>812</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2">
+        <v>14</v>
+      </c>
+      <c r="I3" s="67"/>
+      <c r="J3" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5">
+        <v>812</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="67"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5">
+        <v>822</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2">
+        <v>12</v>
+      </c>
+      <c r="I4" s="67"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="5">
+        <v>822</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="23">
+        <v>12</v>
+      </c>
+      <c r="I5" s="67"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="67"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="I6" s="67"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="67"/>
+      <c r="B7" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2">
+        <v>12</v>
+      </c>
+      <c r="I7" s="67"/>
+      <c r="J7" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="67"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="2">
+        <v>14</v>
+      </c>
+      <c r="I8" s="67"/>
+      <c r="J8" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="67"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="2">
+        <v>14</v>
+      </c>
+      <c r="I9" s="67"/>
+      <c r="J9" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="67"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="2">
+        <v>14</v>
+      </c>
+      <c r="I10" s="67"/>
+      <c r="J10" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="N10" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="67"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="5">
+        <v>822</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2">
+        <v>12</v>
+      </c>
+      <c r="I11" s="67"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="67"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="23">
+        <v>12</v>
+      </c>
+      <c r="I12" s="67"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="67"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="I13" s="67"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="67"/>
+      <c r="B14" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="2">
+        <v>14</v>
+      </c>
+      <c r="I14" s="67"/>
+      <c r="J14" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="N14" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="67"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="2">
+        <v>14</v>
+      </c>
+      <c r="I15" s="67"/>
+      <c r="J15" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="67"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="21">
+        <v>822</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="23">
+        <v>12</v>
+      </c>
+      <c r="I16" s="67"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="23"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="67"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="21">
+        <v>822</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="23">
+        <v>12</v>
+      </c>
+      <c r="I17" s="67"/>
+      <c r="J17" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="21">
+        <v>822</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="N17" s="23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="67"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="I18" s="67"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="67"/>
+      <c r="B19" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="23">
+        <v>14</v>
+      </c>
+      <c r="I19" s="67"/>
+      <c r="J19" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="N19" s="23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="67"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="2">
+        <v>14</v>
+      </c>
+      <c r="I20" s="67"/>
+      <c r="J20" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="N20" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="67"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="21">
+        <v>822</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="23">
+        <v>12</v>
+      </c>
+      <c r="I21" s="67"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="67"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="21">
+        <v>822</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="23">
+        <v>12</v>
+      </c>
+      <c r="I22" s="67"/>
+      <c r="J22" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" s="21">
+        <v>822</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="N22" s="23">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I2:I22"/>
+    <mergeCell ref="A2:A22"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B13:G13"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="中國信託"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3" display="台新銀行"/>
+    <hyperlink ref="C22" r:id="rId4" display="中國信託"/>
+    <hyperlink ref="C11" r:id="rId5" display="中國信託"/>
+    <hyperlink ref="C16" r:id="rId6" display="中國信託"/>
+    <hyperlink ref="C21" r:id="rId7" display="中國信託"/>
+    <hyperlink ref="C12" r:id="rId8" display="中國信託"/>
+    <hyperlink ref="C17" r:id="rId9" display="中國信託"/>
+    <hyperlink ref="C5" r:id="rId10" display="中國信託"/>
+    <hyperlink ref="J2" r:id="rId11" display="台新銀行"/>
+    <hyperlink ref="J7" r:id="rId12"/>
+    <hyperlink ref="J17" r:id="rId13" display="中國信託"/>
+    <hyperlink ref="J22" r:id="rId14" display="中國信託"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId15"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
W315 H1500 - Account (lite), Currency
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="金融簡易版" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Joanna" sheetId="5" r:id="rId2"/>
+    <sheet name="Irving" sheetId="6" r:id="rId3"/>
+    <sheet name="Duncan" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1067,8 +1069,1090 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Bali-ThinkPad</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>臨櫃申請線上約定帳號設定:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>轉帳</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>線上約定帳號設定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>臨櫃申請線上約定帳號設定:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>轉帳</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>線上約定帳號設定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>忽略敦南分行碼:0023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>忽略敦南分行碼:0023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定
+別名設定:
+個人設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>常用帳戶設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>約定帳號</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t xml:space="preserve">網路只可設定非約定
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Bali-ThinkPad</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>臨櫃申請線上約定帳號設定:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>轉帳</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>線上約定帳號設定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>臨櫃申請線上約定帳號設定:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>轉帳</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>線上約定帳號設定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>忽略敦南分行碼:0023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>忽略敦南分行碼:0023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定
+別名設定:
+個人設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>常用帳戶設定</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>/</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>約定帳號</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t xml:space="preserve">網路只可設定非約定
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bali-ThinkPad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路只可設定非約定</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="120">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -1656,7 +2740,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W315 H1400</t>
+    <t>陳美雲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陳美雲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾辰哲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W315 H1500</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1923,7 +3019,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1986,39 +3082,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2035,22 +3110,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2059,15 +3166,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2382,7 +3485,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.05" outlineLevelCol="1"/>
@@ -2416,7 +3519,7 @@
         <v>48</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -2424,58 +3527,58 @@
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:38" ht="16.399999999999999">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="50" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="I3" s="58" t="s">
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="I3" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
       <c r="Q3" s="28"/>
-      <c r="R3" s="59" t="s">
+      <c r="R3" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
       <c r="X3" s="33"/>
-      <c r="Y3" s="48" t="s">
+      <c r="Y3" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="Z3" s="49"/>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="50"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="46"/>
+      <c r="AC3" s="46"/>
+      <c r="AD3" s="46"/>
+      <c r="AE3" s="47"/>
       <c r="AF3" s="33"/>
-      <c r="AG3" s="48" t="s">
+      <c r="AG3" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="AH3" s="49"/>
-      <c r="AI3" s="49"/>
-      <c r="AJ3" s="49"/>
-      <c r="AK3" s="49"/>
-      <c r="AL3" s="50"/>
+      <c r="AH3" s="46"/>
+      <c r="AI3" s="46"/>
+      <c r="AJ3" s="46"/>
+      <c r="AK3" s="46"/>
+      <c r="AL3" s="47"/>
     </row>
     <row r="4" spans="1:38" ht="16.399999999999999">
-      <c r="A4" s="36"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
@@ -2580,19 +3683,19 @@
       </c>
     </row>
     <row r="5" spans="1:38">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:38" ht="16.399999999999999">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="57" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -2612,8 +3715,8 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="16.399999999999999">
-      <c r="A7" s="41"/>
-      <c r="B7" s="44"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="9" t="s">
         <v>33</v>
       </c>
@@ -2632,8 +3735,8 @@
       <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:38" ht="16.399999999999999">
-      <c r="A8" s="41"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
@@ -2651,8 +3754,8 @@
       </c>
     </row>
     <row r="9" spans="1:38" ht="16.399999999999999">
-      <c r="A9" s="41"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="8" t="s">
         <v>26</v>
       </c>
@@ -2670,8 +3773,8 @@
       </c>
     </row>
     <row r="10" spans="1:38" ht="16.399999999999999">
-      <c r="A10" s="41"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="9" t="s">
         <v>22</v>
       </c>
@@ -2694,35 +3797,35 @@
       <c r="M10" s="30"/>
       <c r="N10" s="31"/>
       <c r="O10" s="30"/>
-      <c r="P10" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="T10" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="U10" s="60" t="s">
+      <c r="P10" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="T10" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="U10" s="39" t="s">
         <v>109</v>
       </c>
       <c r="V10" s="30"/>
-      <c r="W10" s="60" t="s">
+      <c r="W10" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AB10" s="30"/>
       <c r="AC10" s="30"/>
       <c r="AD10" s="30"/>
-      <c r="AE10" s="60" t="s">
+      <c r="AE10" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AI10" s="30"/>
       <c r="AJ10" s="30"/>
       <c r="AK10" s="30"/>
-      <c r="AL10" s="60" t="s">
+      <c r="AL10" s="39" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:38" ht="16.399999999999999">
-      <c r="A11" s="41"/>
-      <c r="B11" s="44"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
@@ -2745,35 +3848,35 @@
       <c r="M11" s="30"/>
       <c r="N11" s="31"/>
       <c r="O11" s="30"/>
-      <c r="P11" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="T11" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="U11" s="60" t="s">
+      <c r="P11" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="T11" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="U11" s="39" t="s">
         <v>109</v>
       </c>
       <c r="V11" s="30"/>
-      <c r="W11" s="60" t="s">
+      <c r="W11" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AB11" s="30"/>
       <c r="AC11" s="30"/>
       <c r="AD11" s="30"/>
-      <c r="AE11" s="60" t="s">
+      <c r="AE11" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AI11" s="30"/>
       <c r="AJ11" s="30"/>
       <c r="AK11" s="30"/>
-      <c r="AL11" s="60" t="s">
+      <c r="AL11" s="39" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:38" ht="16.399999999999999">
-      <c r="A12" s="41"/>
-      <c r="B12" s="44"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
@@ -2813,8 +3916,8 @@
       <c r="AL12" s="30"/>
     </row>
     <row r="13" spans="1:38" ht="16.399999999999999">
-      <c r="A13" s="42"/>
-      <c r="B13" s="44"/>
+      <c r="A13" s="56"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="9" t="s">
         <v>98</v>
       </c>
@@ -2854,23 +3957,23 @@
       <c r="AL13" s="30"/>
     </row>
     <row r="14" spans="1:38">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="P14" s="56"/>
-      <c r="W14" s="56"/>
-      <c r="AE14" s="56"/>
-      <c r="AL14" s="56"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="P14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="AE14" s="37"/>
+      <c r="AL14" s="37"/>
     </row>
     <row r="15" spans="1:38" ht="16.399999999999999">
-      <c r="A15" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="57" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -2889,51 +3992,51 @@
         <v>12</v>
       </c>
       <c r="L15" s="30"/>
-      <c r="M15" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="N15" s="60" t="s">
+      <c r="M15" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="N15" s="39" t="s">
         <v>109</v>
       </c>
       <c r="O15" s="30"/>
-      <c r="P15" s="57"/>
-      <c r="S15" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="T15" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="U15" s="60" t="s">
+      <c r="P15" s="38"/>
+      <c r="S15" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="T15" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="U15" s="39" t="s">
         <v>109</v>
       </c>
       <c r="V15" s="30"/>
-      <c r="W15" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB15" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC15" s="60" t="s">
+      <c r="W15" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB15" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC15" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AD15" s="30"/>
-      <c r="AE15" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AI15" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ15" s="60" t="s">
+      <c r="AE15" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI15" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ15" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AK15" s="30"/>
-      <c r="AL15" s="60" t="s">
+      <c r="AL15" s="39" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:38" ht="16.399999999999999">
-      <c r="A16" s="41"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="6" t="s">
         <v>55</v>
       </c>
@@ -2949,14 +4052,14 @@
       <c r="G16" s="2">
         <v>14</v>
       </c>
-      <c r="P16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="AE16" s="56"/>
-      <c r="AL16" s="56"/>
+      <c r="P16" s="37"/>
+      <c r="W16" s="37"/>
+      <c r="AE16" s="37"/>
+      <c r="AL16" s="37"/>
     </row>
     <row r="17" spans="1:38" ht="16.399999999999999">
-      <c r="A17" s="41"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="15" t="s">
         <v>108</v>
       </c>
@@ -2966,64 +4069,64 @@
       <c r="G17" s="2">
         <v>14</v>
       </c>
-      <c r="M17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="N17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="O17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="P17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="R17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="S17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="T17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="U17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="V17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="W17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AI17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK17" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AL17" s="60" t="s">
+      <c r="M17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="N17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="O17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="P17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="R17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="S17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="T17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="U17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="V17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="W17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK17" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL17" s="39" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:38" ht="16.399999999999999">
-      <c r="A18" s="41"/>
-      <c r="B18" s="44"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="15" t="s">
         <v>49</v>
       </c>
@@ -3039,64 +4142,64 @@
       <c r="G18" s="2">
         <v>14</v>
       </c>
-      <c r="M18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="N18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="O18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="P18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="R18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="S18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="T18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="U18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="V18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="W18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AE18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AI18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK18" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AL18" s="60" t="s">
+      <c r="M18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="N18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="O18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="P18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="R18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="S18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="T18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="U18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="V18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="W18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK18" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL18" s="39" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:38" ht="16.399999999999999">
-      <c r="A19" s="41"/>
-      <c r="B19" s="44"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="8" t="s">
         <v>17</v>
       </c>
@@ -3114,49 +4217,49 @@
       </c>
       <c r="I19" s="30"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="60" t="s">
+      <c r="N19" s="39" t="s">
         <v>109</v>
       </c>
       <c r="O19" s="30"/>
       <c r="P19" s="30"/>
-      <c r="R19" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="S19" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="T19" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="U19" s="60" t="s">
+      <c r="R19" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="S19" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="T19" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="U19" s="39" t="s">
         <v>109</v>
       </c>
       <c r="V19" s="30"/>
       <c r="W19" s="30"/>
-      <c r="AB19" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC19" s="60" t="s">
+      <c r="AB19" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC19" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AD19" s="30"/>
-      <c r="AE19" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AI19" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ19" s="60" t="s">
+      <c r="AE19" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI19" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ19" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AK19" s="30"/>
-      <c r="AL19" s="60" t="s">
+      <c r="AL19" s="39" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:38" ht="16.399999999999999">
-      <c r="A20" s="42"/>
-      <c r="B20" s="44"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="9" t="s">
         <v>98</v>
       </c>
@@ -3174,64 +4277,64 @@
       </c>
       <c r="I20" s="30"/>
       <c r="M20" s="30"/>
-      <c r="N20" s="60" t="s">
+      <c r="N20" s="39" t="s">
         <v>109</v>
       </c>
       <c r="O20" s="30"/>
       <c r="P20" s="30"/>
-      <c r="R20" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="S20" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="T20" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="U20" s="60" t="s">
+      <c r="R20" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="S20" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="T20" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="U20" s="39" t="s">
         <v>109</v>
       </c>
       <c r="V20" s="30"/>
       <c r="W20" s="30"/>
-      <c r="AB20" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC20" s="60" t="s">
+      <c r="AB20" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC20" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AD20" s="30"/>
-      <c r="AE20" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AI20" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ20" s="60" t="s">
+      <c r="AE20" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI20" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ20" s="39" t="s">
         <v>109</v>
       </c>
       <c r="AK20" s="30"/>
-      <c r="AL20" s="60" t="s">
+      <c r="AL20" s="39" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:38">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="P21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="AE21" s="56"/>
-      <c r="AL21" s="56"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="P21" s="37"/>
+      <c r="W21" s="37"/>
+      <c r="AE21" s="37"/>
+      <c r="AL21" s="37"/>
     </row>
     <row r="22" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="60" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -3249,13 +4352,13 @@
       <c r="G22" s="23">
         <v>14</v>
       </c>
-      <c r="P22" s="56"/>
-      <c r="W22" s="56"/>
-      <c r="AL22" s="56"/>
+      <c r="P22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="AL22" s="37"/>
     </row>
     <row r="23" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A23" s="46"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="15" t="s">
         <v>55</v>
       </c>
@@ -3271,12 +4374,12 @@
       <c r="G23" s="2">
         <v>14</v>
       </c>
-      <c r="P23" s="56"/>
-      <c r="W23" s="56"/>
+      <c r="P23" s="37"/>
+      <c r="W23" s="37"/>
     </row>
     <row r="24" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A24" s="46"/>
-      <c r="B24" s="37"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="60"/>
       <c r="C24" s="26" t="s">
         <v>74</v>
       </c>
@@ -3292,12 +4395,12 @@
       <c r="G24" s="2">
         <v>14</v>
       </c>
-      <c r="P24" s="56"/>
-      <c r="W24" s="56"/>
+      <c r="P24" s="37"/>
+      <c r="W24" s="37"/>
     </row>
     <row r="25" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A25" s="46"/>
-      <c r="B25" s="37"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="8" t="s">
         <v>26</v>
       </c>
@@ -3313,12 +4416,12 @@
       <c r="G25" s="2">
         <v>13</v>
       </c>
-      <c r="P25" s="56"/>
-      <c r="W25" s="56"/>
+      <c r="P25" s="37"/>
+      <c r="W25" s="37"/>
     </row>
     <row r="26" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A26" s="46"/>
-      <c r="B26" s="37"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="60"/>
       <c r="C26" s="27" t="s">
         <v>77</v>
       </c>
@@ -3334,11 +4437,11 @@
       <c r="G26" s="2">
         <v>13</v>
       </c>
-      <c r="P26" s="56"/>
+      <c r="P26" s="37"/>
     </row>
     <row r="27" spans="1:38" ht="16.399999999999999">
-      <c r="A27" s="46"/>
-      <c r="B27" s="37"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="60"/>
       <c r="C27" s="8" t="s">
         <v>65</v>
       </c>
@@ -3354,11 +4457,22 @@
       <c r="G27" s="2">
         <v>14</v>
       </c>
-      <c r="P27" s="56"/>
+      <c r="M27" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="N27" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="O27" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="P27" s="39" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="28" spans="1:38" ht="16.399999999999999">
-      <c r="A28" s="46"/>
-      <c r="B28" s="37"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="60"/>
       <c r="C28" s="15" t="s">
         <v>49</v>
       </c>
@@ -3374,11 +4488,22 @@
       <c r="G28" s="2">
         <v>14</v>
       </c>
-      <c r="P28" s="56"/>
+      <c r="M28" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="N28" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="O28" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="P28" s="39" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="29" spans="1:38" ht="16.399999999999999">
-      <c r="A29" s="46"/>
-      <c r="B29" s="37"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="60"/>
       <c r="C29" s="8" t="s">
         <v>17</v>
       </c>
@@ -3394,11 +4519,11 @@
       <c r="G29" s="23">
         <v>12</v>
       </c>
-      <c r="P29" s="56"/>
+      <c r="P29" s="37"/>
     </row>
     <row r="30" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A30" s="47"/>
-      <c r="B30" s="37"/>
+      <c r="A30" s="65"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="9" t="s">
         <v>98</v>
       </c>
@@ -3414,23 +4539,23 @@
       <c r="G30" s="23">
         <v>12</v>
       </c>
-      <c r="P30" s="56"/>
+      <c r="P30" s="37"/>
     </row>
     <row r="31" spans="1:38" ht="16.399999999999999">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="P31" s="56"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="P31" s="37"/>
     </row>
     <row r="32" spans="1:38" ht="16.399999999999999">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="60" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -3448,11 +4573,11 @@
       <c r="G32" s="23">
         <v>14</v>
       </c>
-      <c r="P32" s="56"/>
+      <c r="P32" s="37"/>
     </row>
     <row r="33" spans="1:16" ht="16.399999999999999">
-      <c r="A33" s="36"/>
-      <c r="B33" s="37"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="8" t="s">
         <v>86</v>
       </c>
@@ -3468,11 +4593,11 @@
       <c r="G33" s="23">
         <v>13</v>
       </c>
-      <c r="P33" s="56"/>
+      <c r="P33" s="37"/>
     </row>
     <row r="34" spans="1:16" ht="16.399999999999999">
-      <c r="A34" s="36"/>
-      <c r="B34" s="37"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="60"/>
       <c r="C34" s="8" t="s">
         <v>65</v>
       </c>
@@ -3488,11 +4613,11 @@
       <c r="G34" s="23">
         <v>14</v>
       </c>
-      <c r="P34" s="56"/>
+      <c r="P34" s="37"/>
     </row>
     <row r="35" spans="1:16" ht="16.399999999999999">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="60"/>
       <c r="C35" s="15" t="s">
         <v>49</v>
       </c>
@@ -3508,11 +4633,11 @@
       <c r="G35" s="2">
         <v>14</v>
       </c>
-      <c r="P35" s="56"/>
+      <c r="P35" s="37"/>
     </row>
     <row r="36" spans="1:16" ht="16.399999999999999">
-      <c r="A36" s="36"/>
-      <c r="B36" s="37"/>
+      <c r="A36" s="50"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="8" t="s">
         <v>17</v>
       </c>
@@ -3528,11 +4653,11 @@
       <c r="G36" s="23">
         <v>12</v>
       </c>
-      <c r="P36" s="56"/>
+      <c r="P36" s="37"/>
     </row>
     <row r="37" spans="1:16" ht="16.399999999999999">
-      <c r="A37" s="36"/>
-      <c r="B37" s="37"/>
+      <c r="A37" s="50"/>
+      <c r="B37" s="60"/>
       <c r="C37" s="9" t="s">
         <v>98</v>
       </c>
@@ -3548,7 +4673,7 @@
       <c r="G37" s="23">
         <v>12</v>
       </c>
-      <c r="P37" s="56"/>
+      <c r="P37" s="37"/>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="16"/>
@@ -3558,7 +4683,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
-      <c r="P38" s="56"/>
+      <c r="P38" s="37"/>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="17"/>
@@ -3568,21 +4693,29 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
-      <c r="P39" s="56"/>
+      <c r="P39" s="37"/>
     </row>
     <row r="40" spans="1:16">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
-      <c r="P40" s="56"/>
+      <c r="P40" s="37"/>
     </row>
     <row r="41" spans="1:16">
-      <c r="P41" s="56"/>
+      <c r="P41" s="37"/>
     </row>
     <row r="42" spans="1:16">
-      <c r="P42" s="56"/>
+      <c r="P42" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
     <mergeCell ref="R3:W3"/>
     <mergeCell ref="Y3:AE3"/>
     <mergeCell ref="AG3:AL3"/>
@@ -3593,14 +4726,6 @@
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="I3:P3"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3632,7 +4757,7 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.399999999999999"/>
@@ -3646,10 +4771,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="67" t="s">
         <v>113</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -3667,10 +4792,10 @@
       <c r="G2" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="63" t="s">
+      <c r="J2" s="40" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="5">
@@ -3687,8 +4812,8 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
       <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
@@ -3704,8 +4829,8 @@
       <c r="G3" s="2">
         <v>14</v>
       </c>
-      <c r="I3" s="67"/>
-      <c r="J3" s="64" t="s">
+      <c r="I3" s="66"/>
+      <c r="J3" s="41" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="5">
@@ -3722,8 +4847,8 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="67"/>
-      <c r="B4" s="68"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
       <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
@@ -3739,11 +4864,11 @@
       <c r="G4" s="2">
         <v>12</v>
       </c>
-      <c r="I4" s="67"/>
+      <c r="I4" s="66"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="9" t="s">
         <v>98</v>
       </c>
@@ -3759,21 +4884,21 @@
       <c r="G5" s="23">
         <v>12</v>
       </c>
-      <c r="I5" s="67"/>
+      <c r="I5" s="66"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="67"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="I6" s="67"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="I6" s="66"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="67"/>
-      <c r="B7" s="68" t="s">
+      <c r="A7" s="66"/>
+      <c r="B7" s="67" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -3791,8 +4916,8 @@
       <c r="G7" s="2">
         <v>12</v>
       </c>
-      <c r="I7" s="67"/>
-      <c r="J7" s="65" t="s">
+      <c r="I7" s="66"/>
+      <c r="J7" s="42" t="s">
         <v>12</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -3809,8 +4934,8 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="67"/>
-      <c r="B8" s="68"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="6" t="s">
         <v>55</v>
       </c>
@@ -3826,8 +4951,8 @@
       <c r="G8" s="2">
         <v>14</v>
       </c>
-      <c r="I8" s="67"/>
-      <c r="J8" s="65" t="s">
+      <c r="I8" s="66"/>
+      <c r="J8" s="42" t="s">
         <v>55</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -3844,8 +4969,8 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="67"/>
-      <c r="B9" s="68"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="15" t="s">
         <v>108</v>
       </c>
@@ -3855,8 +4980,8 @@
       <c r="G9" s="2">
         <v>14</v>
       </c>
-      <c r="I9" s="67"/>
-      <c r="J9" s="66" t="s">
+      <c r="I9" s="66"/>
+      <c r="J9" s="43" t="s">
         <v>108</v>
       </c>
       <c r="K9" s="5"/>
@@ -3867,8 +4992,8 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="67"/>
-      <c r="B10" s="68"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="15" t="s">
         <v>49</v>
       </c>
@@ -3884,8 +5009,8 @@
       <c r="G10" s="2">
         <v>14</v>
       </c>
-      <c r="I10" s="67"/>
-      <c r="J10" s="66" t="s">
+      <c r="I10" s="66"/>
+      <c r="J10" s="43" t="s">
         <v>49</v>
       </c>
       <c r="K10" s="5" t="s">
@@ -3902,8 +5027,8 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="67"/>
-      <c r="B11" s="68"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
@@ -3919,11 +5044,11 @@
       <c r="G11" s="2">
         <v>12</v>
       </c>
-      <c r="I11" s="67"/>
+      <c r="I11" s="66"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="67"/>
-      <c r="B12" s="68"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="9" t="s">
         <v>98</v>
       </c>
@@ -3939,21 +5064,21 @@
       <c r="G12" s="23">
         <v>12</v>
       </c>
-      <c r="I12" s="67"/>
+      <c r="I12" s="66"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="67"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="I13" s="67"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="I13" s="66"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="67"/>
-      <c r="B14" s="68" t="s">
+      <c r="A14" s="66"/>
+      <c r="B14" s="67" t="s">
         <v>115</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -3971,8 +5096,8 @@
       <c r="G14" s="2">
         <v>14</v>
       </c>
-      <c r="I14" s="67"/>
-      <c r="J14" s="63" t="s">
+      <c r="I14" s="66"/>
+      <c r="J14" s="40" t="s">
         <v>22</v>
       </c>
       <c r="K14" s="21" t="s">
@@ -3989,8 +5114,8 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="67"/>
-      <c r="B15" s="68"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="15" t="s">
         <v>49</v>
       </c>
@@ -4006,8 +5131,8 @@
       <c r="G15" s="2">
         <v>14</v>
       </c>
-      <c r="I15" s="67"/>
-      <c r="J15" s="66" t="s">
+      <c r="I15" s="66"/>
+      <c r="J15" s="43" t="s">
         <v>49</v>
       </c>
       <c r="K15" s="5" t="s">
@@ -4024,8 +5149,8 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="67"/>
-      <c r="B16" s="68"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
@@ -4041,16 +5166,16 @@
       <c r="G16" s="23">
         <v>12</v>
       </c>
-      <c r="I16" s="67"/>
-      <c r="J16" s="63"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="40"/>
       <c r="K16" s="21"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
       <c r="N16" s="23"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="67"/>
-      <c r="B17" s="68"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="9" t="s">
         <v>98</v>
       </c>
@@ -4066,8 +5191,8 @@
       <c r="G17" s="23">
         <v>12</v>
       </c>
-      <c r="I17" s="67"/>
-      <c r="J17" s="63" t="s">
+      <c r="I17" s="66"/>
+      <c r="J17" s="40" t="s">
         <v>98</v>
       </c>
       <c r="K17" s="21">
@@ -4084,18 +5209,18 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="67"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="I18" s="67"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="I18" s="66"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="67"/>
-      <c r="B19" s="68" t="s">
+      <c r="A19" s="66"/>
+      <c r="B19" s="67" t="s">
         <v>114</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -4113,8 +5238,8 @@
       <c r="G19" s="23">
         <v>14</v>
       </c>
-      <c r="I19" s="67"/>
-      <c r="J19" s="63" t="s">
+      <c r="I19" s="66"/>
+      <c r="J19" s="40" t="s">
         <v>22</v>
       </c>
       <c r="K19" s="21" t="s">
@@ -4131,8 +5256,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="67"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="15" t="s">
         <v>49</v>
       </c>
@@ -4148,8 +5273,8 @@
       <c r="G20" s="2">
         <v>14</v>
       </c>
-      <c r="I20" s="67"/>
-      <c r="J20" s="66" t="s">
+      <c r="I20" s="66"/>
+      <c r="J20" s="43" t="s">
         <v>49</v>
       </c>
       <c r="K20" s="5" t="s">
@@ -4166,8 +5291,8 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="67"/>
-      <c r="B21" s="68"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="9" t="s">
         <v>17</v>
       </c>
@@ -4183,16 +5308,16 @@
       <c r="G21" s="23">
         <v>12</v>
       </c>
-      <c r="I21" s="67"/>
-      <c r="J21" s="63"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="40"/>
       <c r="K21" s="21"/>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
       <c r="N21" s="23"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="67"/>
-      <c r="B22" s="68"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="9" t="s">
         <v>98</v>
       </c>
@@ -4208,8 +5333,8 @@
       <c r="G22" s="23">
         <v>12</v>
       </c>
-      <c r="I22" s="67"/>
-      <c r="J22" s="63" t="s">
+      <c r="I22" s="66"/>
+      <c r="J22" s="40" t="s">
         <v>98</v>
       </c>
       <c r="K22" s="21">
@@ -4257,4 +5382,1232 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId15"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:N23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.399999999999999"/>
+  <cols>
+    <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="15.25" customWidth="1"/>
+    <col min="12" max="12" width="10.75" customWidth="1"/>
+    <col min="13" max="13" width="24.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14">
+      <c r="A2" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5">
+        <v>812</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2">
+        <v>14</v>
+      </c>
+      <c r="I2" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="5">
+        <v>812</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5">
+        <v>812</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2">
+        <v>14</v>
+      </c>
+      <c r="I3" s="66"/>
+      <c r="J3" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5">
+        <v>812</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5">
+        <v>822</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2">
+        <v>12</v>
+      </c>
+      <c r="I4" s="66"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="5">
+        <v>822</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="23">
+        <v>12</v>
+      </c>
+      <c r="I5" s="66"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="66"/>
+      <c r="B6" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="I6" s="66"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="66"/>
+      <c r="B7" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="2">
+        <v>14</v>
+      </c>
+      <c r="I7" s="66"/>
+      <c r="J7" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="2">
+        <v>14</v>
+      </c>
+      <c r="I8" s="66"/>
+      <c r="J8" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="N8" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>822</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>12</v>
+      </c>
+      <c r="I9" s="66"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="23">
+        <v>12</v>
+      </c>
+      <c r="I10" s="66"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="66"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="I11" s="66"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="66"/>
+      <c r="B12" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="23">
+        <v>14</v>
+      </c>
+      <c r="I12" s="66"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="66"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="2">
+        <v>14</v>
+      </c>
+      <c r="I13" s="66"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="66"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="2">
+        <v>13</v>
+      </c>
+      <c r="I14" s="66"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="66"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="2">
+        <v>14</v>
+      </c>
+      <c r="I15" s="66"/>
+      <c r="J15" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="N15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="66"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="2">
+        <v>14</v>
+      </c>
+      <c r="I16" s="66"/>
+      <c r="J16" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="N16" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="66"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="21">
+        <v>822</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="23">
+        <v>12</v>
+      </c>
+      <c r="I17" s="66"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="23"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="66"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="21">
+        <v>822</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="23">
+        <v>12</v>
+      </c>
+      <c r="I18" s="66"/>
+      <c r="J18" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" s="21">
+        <v>822</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="N18" s="23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="66"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="I19" s="66"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="66"/>
+      <c r="B20" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="23">
+        <v>14</v>
+      </c>
+      <c r="I20" s="66"/>
+      <c r="J20" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="N20" s="23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="66"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="2">
+        <v>14</v>
+      </c>
+      <c r="I21" s="66"/>
+      <c r="J21" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M21" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="N21" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="66"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="21">
+        <v>822</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="23">
+        <v>12</v>
+      </c>
+      <c r="I22" s="66"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="23"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="66"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="21">
+        <v>822</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="23">
+        <v>12</v>
+      </c>
+      <c r="I23" s="66"/>
+      <c r="J23" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="K23" s="21">
+        <v>822</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="N23" s="23">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="I2:I23"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B12:B18"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="中國信託"/>
+    <hyperlink ref="C2" r:id="rId2" display="台新銀行"/>
+    <hyperlink ref="C23" r:id="rId3" display="中國信託"/>
+    <hyperlink ref="C9" r:id="rId4" display="中國信託"/>
+    <hyperlink ref="C17" r:id="rId5" display="中國信託"/>
+    <hyperlink ref="C22" r:id="rId6" display="中國信託"/>
+    <hyperlink ref="C10" r:id="rId7" display="中國信託"/>
+    <hyperlink ref="C18" r:id="rId8" display="中國信託"/>
+    <hyperlink ref="C5" r:id="rId9" display="中國信託"/>
+    <hyperlink ref="J2" r:id="rId10" display="台新銀行"/>
+    <hyperlink ref="J18" r:id="rId11" display="中國信託"/>
+    <hyperlink ref="J23" r:id="rId12" display="中國信託"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:N22"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.399999999999999"/>
+  <cols>
+    <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="15.25" customWidth="1"/>
+    <col min="12" max="12" width="10.75" customWidth="1"/>
+    <col min="13" max="13" width="24.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14">
+      <c r="A2" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5">
+        <v>812</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2">
+        <v>14</v>
+      </c>
+      <c r="I2" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="5">
+        <v>812</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5">
+        <v>812</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2">
+        <v>14</v>
+      </c>
+      <c r="I3" s="66"/>
+      <c r="J3" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="5">
+        <v>812</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5">
+        <v>822</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2">
+        <v>12</v>
+      </c>
+      <c r="I4" s="66"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="5">
+        <v>822</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="23">
+        <v>12</v>
+      </c>
+      <c r="I5" s="66"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="66"/>
+      <c r="B6" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="I6" s="66"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="66"/>
+      <c r="B7" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="2">
+        <v>14</v>
+      </c>
+      <c r="I7" s="66"/>
+      <c r="J7" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="2">
+        <v>14</v>
+      </c>
+      <c r="I8" s="66"/>
+      <c r="J8" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="N8" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>822</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>12</v>
+      </c>
+      <c r="I9" s="66"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="23">
+        <v>12</v>
+      </c>
+      <c r="I10" s="66"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="66"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="I11" s="66"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="66"/>
+      <c r="B12" s="70" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="2">
+        <v>14</v>
+      </c>
+      <c r="I12" s="66"/>
+      <c r="J12" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="N12" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="66"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="2">
+        <v>14</v>
+      </c>
+      <c r="I13" s="66"/>
+      <c r="J13" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="66"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="21">
+        <v>822</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="23">
+        <v>12</v>
+      </c>
+      <c r="I14" s="66"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="66"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="21">
+        <v>822</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="23">
+        <v>12</v>
+      </c>
+      <c r="I15" s="66"/>
+      <c r="J15" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="21">
+        <v>822</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="N15" s="23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="66"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="I16" s="66"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="66"/>
+      <c r="B17" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="23">
+        <v>14</v>
+      </c>
+      <c r="I17" s="66"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="66"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="23">
+        <v>13</v>
+      </c>
+      <c r="I18" s="66"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="66"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="23">
+        <v>14</v>
+      </c>
+      <c r="I19" s="66"/>
+      <c r="J19" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="N19" s="23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="66"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="2">
+        <v>14</v>
+      </c>
+      <c r="I20" s="66"/>
+      <c r="J20" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="N20" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="66"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="21">
+        <v>822</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="23">
+        <v>12</v>
+      </c>
+      <c r="I21" s="66"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="66"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="21">
+        <v>822</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="23">
+        <v>12</v>
+      </c>
+      <c r="I22" s="66"/>
+      <c r="J22" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" s="21">
+        <v>822</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="N22" s="23">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A2:A22"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="I2:I22"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:B22"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="中國信託"/>
+    <hyperlink ref="C2" r:id="rId2" display="台新銀行"/>
+    <hyperlink ref="C22" r:id="rId3" display="中國信託"/>
+    <hyperlink ref="C9" r:id="rId4" display="中國信託"/>
+    <hyperlink ref="C14" r:id="rId5" display="中國信託"/>
+    <hyperlink ref="C21" r:id="rId6" display="中國信託"/>
+    <hyperlink ref="C10" r:id="rId7" display="中國信託"/>
+    <hyperlink ref="C15" r:id="rId8" display="中國信託"/>
+    <hyperlink ref="C5" r:id="rId9" display="中國信託"/>
+    <hyperlink ref="J2" r:id="rId10" display="台新銀行"/>
+    <hyperlink ref="J15" r:id="rId11" display="中國信託"/>
+    <hyperlink ref="J22" r:id="rId12" display="中國信託"/>
+    <hyperlink ref="C18" r:id="rId13"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
W322 H1000 - Account, Account (lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="419" yWindow="105" windowWidth="16979" windowHeight="6336"/>
+    <workbookView xWindow="419" yWindow="105" windowWidth="16979" windowHeight="6336" tabRatio="508"/>
   </bookViews>
   <sheets>
     <sheet name="金融簡易版" sheetId="4" r:id="rId1"/>
@@ -417,6 +417,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="C15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Bali-ThinkPad:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="細明體"/>
+            <family val="3"/>
+            <charset val="136"/>
+          </rPr>
+          <t>網路可設定約定及非約定
+需金融卡認證</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C19" authorId="0">
       <text>
         <r>
@@ -2216,7 +2242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="127">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -2844,7 +2870,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>W321 H1630</t>
+    <t>W322 H1000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3214,38 +3240,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3265,15 +3260,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3292,9 +3321,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3651,58 +3677,58 @@
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:38" ht="16.399999999999999">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="55" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="I3" s="69" t="s">
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="I3" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
       <c r="Q3" s="28"/>
-      <c r="R3" s="60" t="s">
+      <c r="R3" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="60"/>
-      <c r="W3" s="60"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
       <c r="X3" s="33"/>
-      <c r="Y3" s="61" t="s">
+      <c r="Y3" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="Z3" s="62"/>
-      <c r="AA3" s="62"/>
-      <c r="AB3" s="62"/>
-      <c r="AC3" s="62"/>
-      <c r="AD3" s="62"/>
-      <c r="AE3" s="63"/>
+      <c r="Z3" s="51"/>
+      <c r="AA3" s="51"/>
+      <c r="AB3" s="51"/>
+      <c r="AC3" s="51"/>
+      <c r="AD3" s="51"/>
+      <c r="AE3" s="52"/>
       <c r="AF3" s="33"/>
-      <c r="AG3" s="61" t="s">
+      <c r="AG3" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="AH3" s="62"/>
-      <c r="AI3" s="62"/>
-      <c r="AJ3" s="62"/>
-      <c r="AK3" s="62"/>
-      <c r="AL3" s="63"/>
+      <c r="AH3" s="51"/>
+      <c r="AI3" s="51"/>
+      <c r="AJ3" s="51"/>
+      <c r="AK3" s="51"/>
+      <c r="AL3" s="52"/>
     </row>
     <row r="4" spans="1:38" ht="16.399999999999999">
-      <c r="A4" s="48"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="11" t="s">
         <v>44</v>
       </c>
@@ -3807,19 +3833,19 @@
       </c>
     </row>
     <row r="5" spans="1:38">
-      <c r="A5" s="67"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
     </row>
     <row r="6" spans="1:38" ht="16.399999999999999">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="62" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -3845,8 +3871,8 @@
       <c r="O6" s="30"/>
     </row>
     <row r="7" spans="1:38" ht="16.399999999999999">
-      <c r="A7" s="53"/>
-      <c r="B7" s="56"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="9" t="s">
         <v>32</v>
       </c>
@@ -3918,8 +3944,8 @@
       </c>
     </row>
     <row r="8" spans="1:38" ht="16.399999999999999">
-      <c r="A8" s="53"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
@@ -3937,8 +3963,8 @@
       </c>
     </row>
     <row r="9" spans="1:38" ht="16.399999999999999">
-      <c r="A9" s="53"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
@@ -3956,8 +3982,8 @@
       </c>
     </row>
     <row r="10" spans="1:38" ht="16.399999999999999">
-      <c r="A10" s="53"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
@@ -4007,8 +4033,8 @@
       </c>
     </row>
     <row r="11" spans="1:38" ht="16.399999999999999">
-      <c r="A11" s="53"/>
-      <c r="B11" s="56"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
@@ -4058,8 +4084,8 @@
       </c>
     </row>
     <row r="12" spans="1:38" ht="16.399999999999999">
-      <c r="A12" s="53"/>
-      <c r="B12" s="56"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
@@ -4101,8 +4127,8 @@
       <c r="AL12" s="30"/>
     </row>
     <row r="13" spans="1:38" ht="16.399999999999999">
-      <c r="A13" s="54"/>
-      <c r="B13" s="56"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="9" t="s">
         <v>97</v>
       </c>
@@ -4144,27 +4170,27 @@
       <c r="AL13" s="30"/>
     </row>
     <row r="14" spans="1:38">
-      <c r="A14" s="50"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
       <c r="P14" s="37"/>
       <c r="W14" s="37"/>
       <c r="AE14" s="37"/>
       <c r="AL14" s="37"/>
     </row>
     <row r="15" spans="1:38" ht="16.399999999999999">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>11</v>
+      <c r="C15" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="44" t="s">
         <v>119</v>
@@ -4178,23 +4204,13 @@
       <c r="G15" s="2">
         <v>12</v>
       </c>
-      <c r="J15" s="38" t="s">
-        <v>108</v>
-      </c>
+      <c r="J15" s="30"/>
       <c r="L15" s="30"/>
-      <c r="M15" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="N15" s="38" t="s">
-        <v>108</v>
-      </c>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
       <c r="O15" s="30"/>
-      <c r="P15" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="S15" s="38" t="s">
-        <v>108</v>
-      </c>
+      <c r="P15" s="30"/>
+      <c r="S15" s="30"/>
       <c r="T15" s="38" t="s">
         <v>108</v>
       </c>
@@ -4202,9 +4218,7 @@
         <v>108</v>
       </c>
       <c r="V15" s="30"/>
-      <c r="W15" s="38" t="s">
-        <v>108</v>
-      </c>
+      <c r="W15" s="30"/>
       <c r="AB15" s="38" t="s">
         <v>108</v>
       </c>
@@ -4212,9 +4226,7 @@
         <v>108</v>
       </c>
       <c r="AD15" s="30"/>
-      <c r="AE15" s="38" t="s">
-        <v>108</v>
-      </c>
+      <c r="AE15" s="30"/>
       <c r="AI15" s="38" t="s">
         <v>108</v>
       </c>
@@ -4222,21 +4234,19 @@
         <v>108</v>
       </c>
       <c r="AK15" s="30"/>
-      <c r="AL15" s="38" t="s">
-        <v>108</v>
-      </c>
+      <c r="AL15" s="30"/>
     </row>
     <row r="16" spans="1:38" ht="16.399999999999999">
-      <c r="A16" s="53"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="6" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>56</v>
+      <c r="E16" s="45" t="s">
+        <v>9</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>57</v>
@@ -4250,8 +4260,8 @@
       <c r="AL16" s="37"/>
     </row>
     <row r="17" spans="1:38" ht="16.399999999999999">
-      <c r="A17" s="53"/>
-      <c r="B17" s="56"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="15" t="s">
         <v>107</v>
       </c>
@@ -4317,8 +4327,8 @@
       </c>
     </row>
     <row r="18" spans="1:38" ht="16.399999999999999">
-      <c r="A18" s="53"/>
-      <c r="B18" s="56"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="15" t="s">
         <v>48</v>
       </c>
@@ -4390,8 +4400,8 @@
       </c>
     </row>
     <row r="19" spans="1:38" ht="16.399999999999999">
-      <c r="A19" s="53"/>
-      <c r="B19" s="56"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
@@ -4450,8 +4460,8 @@
       </c>
     </row>
     <row r="20" spans="1:38" ht="16.399999999999999">
-      <c r="A20" s="54"/>
-      <c r="B20" s="56"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="9" t="s">
         <v>97</v>
       </c>
@@ -4510,23 +4520,23 @@
       </c>
     </row>
     <row r="21" spans="1:38">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
       <c r="P21" s="37"/>
       <c r="W21" s="37"/>
       <c r="AE21" s="37"/>
       <c r="AL21" s="37"/>
     </row>
     <row r="22" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="65" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -4549,8 +4559,8 @@
       <c r="AL22" s="37"/>
     </row>
     <row r="23" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A23" s="58"/>
-      <c r="B23" s="49"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="15" t="s">
         <v>54</v>
       </c>
@@ -4570,8 +4580,8 @@
       <c r="W23" s="37"/>
     </row>
     <row r="24" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A24" s="58"/>
-      <c r="B24" s="49"/>
+      <c r="A24" s="69"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="26" t="s">
         <v>73</v>
       </c>
@@ -4591,8 +4601,8 @@
       <c r="W24" s="37"/>
     </row>
     <row r="25" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A25" s="58"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="8" t="s">
         <v>25</v>
       </c>
@@ -4612,8 +4622,8 @@
       <c r="W25" s="37"/>
     </row>
     <row r="26" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A26" s="58"/>
-      <c r="B26" s="49"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="27" t="s">
         <v>76</v>
       </c>
@@ -4632,8 +4642,8 @@
       <c r="P26" s="37"/>
     </row>
     <row r="27" spans="1:38" ht="16.399999999999999">
-      <c r="A27" s="58"/>
-      <c r="B27" s="49"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="8" t="s">
         <v>64</v>
       </c>
@@ -4663,8 +4673,8 @@
       </c>
     </row>
     <row r="28" spans="1:38" ht="16.399999999999999">
-      <c r="A28" s="58"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
@@ -4694,8 +4704,8 @@
       </c>
     </row>
     <row r="29" spans="1:38" ht="16.399999999999999">
-      <c r="A29" s="58"/>
-      <c r="B29" s="49"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="65"/>
       <c r="C29" s="8" t="s">
         <v>16</v>
       </c>
@@ -4714,8 +4724,8 @@
       <c r="P29" s="37"/>
     </row>
     <row r="30" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A30" s="59"/>
-      <c r="B30" s="49"/>
+      <c r="A30" s="70"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="9" t="s">
         <v>97</v>
       </c>
@@ -4734,20 +4744,20 @@
       <c r="P30" s="37"/>
     </row>
     <row r="31" spans="1:38" ht="16.399999999999999">
-      <c r="A31" s="64"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
+      <c r="A31" s="53"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
       <c r="P31" s="37"/>
     </row>
     <row r="32" spans="1:38" ht="16.399999999999999">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="65" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -4768,8 +4778,8 @@
       <c r="P32" s="37"/>
     </row>
     <row r="33" spans="1:38" ht="16.399999999999999">
-      <c r="A33" s="48"/>
-      <c r="B33" s="49"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="8" t="s">
         <v>85</v>
       </c>
@@ -4790,8 +4800,8 @@
       <c r="AK33" s="30"/>
     </row>
     <row r="34" spans="1:38" ht="16.399999999999999">
-      <c r="A34" s="48"/>
-      <c r="B34" s="49"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="65"/>
       <c r="C34" s="8" t="s">
         <v>64</v>
       </c>
@@ -4822,8 +4832,8 @@
       <c r="AK34" s="30"/>
     </row>
     <row r="35" spans="1:38" ht="16.399999999999999">
-      <c r="A35" s="48"/>
-      <c r="B35" s="49"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="65"/>
       <c r="C35" s="15" t="s">
         <v>48</v>
       </c>
@@ -4842,8 +4852,8 @@
       <c r="P35" s="37"/>
     </row>
     <row r="36" spans="1:38" ht="16.399999999999999">
-      <c r="A36" s="48"/>
-      <c r="B36" s="49"/>
+      <c r="A36" s="55"/>
+      <c r="B36" s="65"/>
       <c r="C36" s="8" t="s">
         <v>16</v>
       </c>
@@ -4867,8 +4877,8 @@
       <c r="AL36" s="30"/>
     </row>
     <row r="37" spans="1:38" ht="16.399999999999999">
-      <c r="A37" s="48"/>
-      <c r="B37" s="49"/>
+      <c r="A37" s="55"/>
+      <c r="B37" s="65"/>
       <c r="C37" s="9" t="s">
         <v>97</v>
       </c>
@@ -4924,6 +4934,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
     <mergeCell ref="R3:W3"/>
     <mergeCell ref="Y3:AE3"/>
     <mergeCell ref="AG3:AL3"/>
@@ -4934,37 +4952,28 @@
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="I3:P3"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C6" r:id="rId1" display="台灣營行"/>
-    <hyperlink ref="C15" r:id="rId2"/>
-    <hyperlink ref="C10" r:id="rId3" display="台新銀行"/>
-    <hyperlink ref="C8" r:id="rId4" display="國泰世華"/>
-    <hyperlink ref="C9" r:id="rId5"/>
-    <hyperlink ref="C25" r:id="rId6"/>
-    <hyperlink ref="C37" r:id="rId7" display="中國信託"/>
-    <hyperlink ref="C33" r:id="rId8"/>
-    <hyperlink ref="C19" r:id="rId9" display="中國信託"/>
-    <hyperlink ref="C29" r:id="rId10" display="中國信託"/>
-    <hyperlink ref="C36" r:id="rId11" display="中國信託"/>
-    <hyperlink ref="C20" r:id="rId12" display="中國信託"/>
-    <hyperlink ref="C30" r:id="rId13" display="中國信託"/>
-    <hyperlink ref="C12" r:id="rId14" display="中國信託"/>
-    <hyperlink ref="C13" r:id="rId15" display="中國信託"/>
+    <hyperlink ref="C10" r:id="rId2" display="台新銀行"/>
+    <hyperlink ref="C8" r:id="rId3" display="國泰世華"/>
+    <hyperlink ref="C9" r:id="rId4"/>
+    <hyperlink ref="C25" r:id="rId5"/>
+    <hyperlink ref="C37" r:id="rId6" display="中國信託"/>
+    <hyperlink ref="C33" r:id="rId7"/>
+    <hyperlink ref="C19" r:id="rId8" display="中國信託"/>
+    <hyperlink ref="C29" r:id="rId9" display="中國信託"/>
+    <hyperlink ref="C36" r:id="rId10" display="中國信託"/>
+    <hyperlink ref="C20" r:id="rId11" display="中國信託"/>
+    <hyperlink ref="C30" r:id="rId12" display="中國信託"/>
+    <hyperlink ref="C12" r:id="rId13" display="中國信託"/>
+    <hyperlink ref="C13" r:id="rId14" display="中國信託"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="4294967293" r:id="rId15"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId17"/>
+  <legacyDrawing r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -4987,10 +4996,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -5008,7 +5017,7 @@
       <c r="G2" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="71" t="s">
         <v>93</v>
       </c>
       <c r="J2" s="39" t="s">
@@ -5028,8 +5037,8 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="70"/>
-      <c r="B3" s="71"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
@@ -5045,7 +5054,7 @@
       <c r="G3" s="2">
         <v>14</v>
       </c>
-      <c r="I3" s="70"/>
+      <c r="I3" s="71"/>
       <c r="J3" s="40" t="s">
         <v>19</v>
       </c>
@@ -5063,8 +5072,8 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="70"/>
-      <c r="B4" s="71"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -5080,11 +5089,11 @@
       <c r="G4" s="2">
         <v>12</v>
       </c>
-      <c r="I4" s="70"/>
+      <c r="I4" s="71"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="9" t="s">
         <v>97</v>
       </c>
@@ -5100,21 +5109,21 @@
       <c r="G5" s="23">
         <v>12</v>
       </c>
-      <c r="I5" s="70"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="70"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="I6" s="70"/>
+      <c r="A6" s="71"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="I6" s="71"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="70"/>
-      <c r="B7" s="71" t="s">
+      <c r="A7" s="71"/>
+      <c r="B7" s="72" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -5126,13 +5135,13 @@
       <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="48" t="s">
         <v>125</v>
       </c>
       <c r="G7" s="2">
         <v>12</v>
       </c>
-      <c r="I7" s="70"/>
+      <c r="I7" s="71"/>
       <c r="J7" s="41" t="s">
         <v>11</v>
       </c>
@@ -5142,7 +5151,7 @@
       <c r="L7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="76" t="s">
+      <c r="M7" s="48" t="s">
         <v>125</v>
       </c>
       <c r="N7" s="2">
@@ -5150,8 +5159,8 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="70"/>
-      <c r="B8" s="71"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="6" t="s">
         <v>54</v>
       </c>
@@ -5167,7 +5176,7 @@
       <c r="G8" s="2">
         <v>14</v>
       </c>
-      <c r="I8" s="70"/>
+      <c r="I8" s="71"/>
       <c r="J8" s="41" t="s">
         <v>54</v>
       </c>
@@ -5185,8 +5194,8 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="70"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="15" t="s">
         <v>107</v>
       </c>
@@ -5196,7 +5205,7 @@
       <c r="G9" s="2">
         <v>14</v>
       </c>
-      <c r="I9" s="70"/>
+      <c r="I9" s="71"/>
       <c r="J9" s="42" t="s">
         <v>107</v>
       </c>
@@ -5208,8 +5217,8 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="70"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="15" t="s">
         <v>48</v>
       </c>
@@ -5225,7 +5234,7 @@
       <c r="G10" s="2">
         <v>14</v>
       </c>
-      <c r="I10" s="70"/>
+      <c r="I10" s="71"/>
       <c r="J10" s="42" t="s">
         <v>48</v>
       </c>
@@ -5243,8 +5252,8 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="70"/>
-      <c r="B11" s="71"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
@@ -5260,11 +5269,11 @@
       <c r="G11" s="2">
         <v>12</v>
       </c>
-      <c r="I11" s="70"/>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="70"/>
-      <c r="B12" s="71"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="9" t="s">
         <v>97</v>
       </c>
@@ -5280,21 +5289,21 @@
       <c r="G12" s="23">
         <v>12</v>
       </c>
-      <c r="I12" s="70"/>
+      <c r="I12" s="71"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="70"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="I13" s="70"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="I13" s="71"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="70"/>
-      <c r="B14" s="71" t="s">
+      <c r="A14" s="71"/>
+      <c r="B14" s="72" t="s">
         <v>114</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -5312,7 +5321,7 @@
       <c r="G14" s="2">
         <v>14</v>
       </c>
-      <c r="I14" s="70"/>
+      <c r="I14" s="71"/>
       <c r="J14" s="39" t="s">
         <v>21</v>
       </c>
@@ -5330,8 +5339,8 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="70"/>
-      <c r="B15" s="71"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="15" t="s">
         <v>48</v>
       </c>
@@ -5347,7 +5356,7 @@
       <c r="G15" s="2">
         <v>14</v>
       </c>
-      <c r="I15" s="70"/>
+      <c r="I15" s="71"/>
       <c r="J15" s="42" t="s">
         <v>48</v>
       </c>
@@ -5365,8 +5374,8 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="70"/>
-      <c r="B16" s="71"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="9" t="s">
         <v>16</v>
       </c>
@@ -5382,7 +5391,7 @@
       <c r="G16" s="23">
         <v>12</v>
       </c>
-      <c r="I16" s="70"/>
+      <c r="I16" s="71"/>
       <c r="J16" s="39"/>
       <c r="K16" s="21"/>
       <c r="L16" s="22"/>
@@ -5390,8 +5399,8 @@
       <c r="N16" s="23"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="70"/>
-      <c r="B17" s="71"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="9" t="s">
         <v>97</v>
       </c>
@@ -5407,7 +5416,7 @@
       <c r="G17" s="23">
         <v>12</v>
       </c>
-      <c r="I17" s="70"/>
+      <c r="I17" s="71"/>
       <c r="J17" s="39" t="s">
         <v>97</v>
       </c>
@@ -5425,18 +5434,18 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="70"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="I18" s="70"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="I18" s="71"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="70"/>
-      <c r="B19" s="71" t="s">
+      <c r="A19" s="71"/>
+      <c r="B19" s="72" t="s">
         <v>113</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -5454,7 +5463,7 @@
       <c r="G19" s="23">
         <v>14</v>
       </c>
-      <c r="I19" s="70"/>
+      <c r="I19" s="71"/>
       <c r="J19" s="39" t="s">
         <v>21</v>
       </c>
@@ -5472,8 +5481,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="70"/>
-      <c r="B20" s="71"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="15" t="s">
         <v>48</v>
       </c>
@@ -5489,7 +5498,7 @@
       <c r="G20" s="2">
         <v>14</v>
       </c>
-      <c r="I20" s="70"/>
+      <c r="I20" s="71"/>
       <c r="J20" s="42" t="s">
         <v>48</v>
       </c>
@@ -5507,8 +5516,8 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="70"/>
-      <c r="B21" s="71"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="9" t="s">
         <v>16</v>
       </c>
@@ -5524,7 +5533,7 @@
       <c r="G21" s="23">
         <v>12</v>
       </c>
-      <c r="I21" s="70"/>
+      <c r="I21" s="71"/>
       <c r="J21" s="39"/>
       <c r="K21" s="21"/>
       <c r="L21" s="22"/>
@@ -5532,8 +5541,8 @@
       <c r="N21" s="23"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="70"/>
-      <c r="B22" s="71"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="9" t="s">
         <v>97</v>
       </c>
@@ -5549,7 +5558,7 @@
       <c r="G22" s="23">
         <v>12</v>
       </c>
-      <c r="I22" s="70"/>
+      <c r="I22" s="71"/>
       <c r="J22" s="39" t="s">
         <v>97</v>
       </c>
@@ -5619,10 +5628,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -5640,7 +5649,7 @@
       <c r="G2" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="71" t="s">
         <v>93</v>
       </c>
       <c r="J2" s="39" t="s">
@@ -5660,8 +5669,8 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="70"/>
-      <c r="B3" s="71"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
@@ -5677,7 +5686,7 @@
       <c r="G3" s="2">
         <v>14</v>
       </c>
-      <c r="I3" s="70"/>
+      <c r="I3" s="71"/>
       <c r="J3" s="40" t="s">
         <v>19</v>
       </c>
@@ -5695,8 +5704,8 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="70"/>
-      <c r="B4" s="71"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -5712,11 +5721,11 @@
       <c r="G4" s="2">
         <v>12</v>
       </c>
-      <c r="I4" s="70"/>
+      <c r="I4" s="71"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="9" t="s">
         <v>97</v>
       </c>
@@ -5732,21 +5741,21 @@
       <c r="G5" s="23">
         <v>12</v>
       </c>
-      <c r="I5" s="70"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="70"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="I6" s="70"/>
+      <c r="A6" s="71"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="I6" s="71"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="70"/>
-      <c r="B7" s="71" t="s">
+      <c r="A7" s="71"/>
+      <c r="B7" s="72" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -5758,7 +5767,7 @@
       <c r="G7" s="2">
         <v>14</v>
       </c>
-      <c r="I7" s="70"/>
+      <c r="I7" s="71"/>
       <c r="J7" s="42" t="s">
         <v>107</v>
       </c>
@@ -5770,8 +5779,8 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="70"/>
-      <c r="B8" s="71"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="15" t="s">
         <v>48</v>
       </c>
@@ -5787,7 +5796,7 @@
       <c r="G8" s="2">
         <v>14</v>
       </c>
-      <c r="I8" s="70"/>
+      <c r="I8" s="71"/>
       <c r="J8" s="42" t="s">
         <v>48</v>
       </c>
@@ -5805,8 +5814,8 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="70"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -5822,11 +5831,11 @@
       <c r="G9" s="2">
         <v>12</v>
       </c>
-      <c r="I9" s="70"/>
+      <c r="I9" s="71"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="70"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="9" t="s">
         <v>97</v>
       </c>
@@ -5842,21 +5851,21 @@
       <c r="G10" s="23">
         <v>12</v>
       </c>
-      <c r="I10" s="70"/>
+      <c r="I10" s="71"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="70"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="I11" s="70"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="70"/>
-      <c r="B12" s="57" t="s">
+      <c r="A12" s="71"/>
+      <c r="B12" s="68" t="s">
         <v>114</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -5874,11 +5883,11 @@
       <c r="G12" s="23">
         <v>14</v>
       </c>
-      <c r="I12" s="70"/>
+      <c r="I12" s="71"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="70"/>
-      <c r="B13" s="74"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="15" t="s">
         <v>54</v>
       </c>
@@ -5894,11 +5903,11 @@
       <c r="G13" s="2">
         <v>14</v>
       </c>
-      <c r="I13" s="70"/>
+      <c r="I13" s="71"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="70"/>
-      <c r="B14" s="74"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
@@ -5914,11 +5923,11 @@
       <c r="G14" s="2">
         <v>13</v>
       </c>
-      <c r="I14" s="70"/>
+      <c r="I14" s="71"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="70"/>
-      <c r="B15" s="74"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="9" t="s">
         <v>21</v>
       </c>
@@ -5934,7 +5943,7 @@
       <c r="G15" s="2">
         <v>14</v>
       </c>
-      <c r="I15" s="70"/>
+      <c r="I15" s="71"/>
       <c r="J15" s="39" t="s">
         <v>21</v>
       </c>
@@ -5952,8 +5961,8 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="70"/>
-      <c r="B16" s="74"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="15" t="s">
         <v>48</v>
       </c>
@@ -5969,7 +5978,7 @@
       <c r="G16" s="2">
         <v>14</v>
       </c>
-      <c r="I16" s="70"/>
+      <c r="I16" s="71"/>
       <c r="J16" s="42" t="s">
         <v>48</v>
       </c>
@@ -5987,8 +5996,8 @@
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="70"/>
-      <c r="B17" s="74"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
@@ -6004,7 +6013,7 @@
       <c r="G17" s="23">
         <v>12</v>
       </c>
-      <c r="I17" s="70"/>
+      <c r="I17" s="71"/>
       <c r="J17" s="39"/>
       <c r="K17" s="21"/>
       <c r="L17" s="22"/>
@@ -6012,8 +6021,8 @@
       <c r="N17" s="23"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="70"/>
-      <c r="B18" s="75"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="76"/>
       <c r="C18" s="9" t="s">
         <v>97</v>
       </c>
@@ -6029,7 +6038,7 @@
       <c r="G18" s="23">
         <v>12</v>
       </c>
-      <c r="I18" s="70"/>
+      <c r="I18" s="71"/>
       <c r="J18" s="39" t="s">
         <v>97</v>
       </c>
@@ -6047,18 +6056,18 @@
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="70"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="I19" s="70"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="I19" s="71"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="70"/>
-      <c r="B20" s="71" t="s">
+      <c r="A20" s="71"/>
+      <c r="B20" s="72" t="s">
         <v>113</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -6076,7 +6085,7 @@
       <c r="G20" s="23">
         <v>14</v>
       </c>
-      <c r="I20" s="70"/>
+      <c r="I20" s="71"/>
       <c r="J20" s="39" t="s">
         <v>21</v>
       </c>
@@ -6094,8 +6103,8 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="70"/>
-      <c r="B21" s="71"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="15" t="s">
         <v>48</v>
       </c>
@@ -6111,7 +6120,7 @@
       <c r="G21" s="2">
         <v>14</v>
       </c>
-      <c r="I21" s="70"/>
+      <c r="I21" s="71"/>
       <c r="J21" s="42" t="s">
         <v>48</v>
       </c>
@@ -6129,8 +6138,8 @@
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="70"/>
-      <c r="B22" s="71"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="9" t="s">
         <v>16</v>
       </c>
@@ -6146,7 +6155,7 @@
       <c r="G22" s="23">
         <v>12</v>
       </c>
-      <c r="I22" s="70"/>
+      <c r="I22" s="71"/>
       <c r="J22" s="39"/>
       <c r="K22" s="21"/>
       <c r="L22" s="22"/>
@@ -6154,8 +6163,8 @@
       <c r="N22" s="23"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="70"/>
-      <c r="B23" s="71"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="72"/>
       <c r="C23" s="9" t="s">
         <v>97</v>
       </c>
@@ -6171,7 +6180,7 @@
       <c r="G23" s="23">
         <v>12</v>
       </c>
-      <c r="I23" s="70"/>
+      <c r="I23" s="71"/>
       <c r="J23" s="39" t="s">
         <v>97</v>
       </c>
@@ -6227,7 +6236,7 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.399999999999999"/>
@@ -6241,10 +6250,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -6262,7 +6271,7 @@
       <c r="G2" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="71" t="s">
         <v>93</v>
       </c>
       <c r="J2" s="39" t="s">
@@ -6282,8 +6291,8 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="70"/>
-      <c r="B3" s="71"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
@@ -6299,7 +6308,7 @@
       <c r="G3" s="2">
         <v>14</v>
       </c>
-      <c r="I3" s="70"/>
+      <c r="I3" s="71"/>
       <c r="J3" s="40" t="s">
         <v>19</v>
       </c>
@@ -6317,8 +6326,8 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="70"/>
-      <c r="B4" s="71"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -6334,11 +6343,11 @@
       <c r="G4" s="2">
         <v>12</v>
       </c>
-      <c r="I4" s="70"/>
+      <c r="I4" s="71"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="9" t="s">
         <v>97</v>
       </c>
@@ -6354,23 +6363,23 @@
       <c r="G5" s="23">
         <v>12</v>
       </c>
-      <c r="I5" s="70"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="70"/>
-      <c r="B6" s="50" t="s">
+      <c r="A6" s="71"/>
+      <c r="B6" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="I6" s="70"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="I6" s="71"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="70"/>
-      <c r="B7" s="71" t="s">
+      <c r="A7" s="71"/>
+      <c r="B7" s="72" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -6382,7 +6391,7 @@
       <c r="G7" s="2">
         <v>14</v>
       </c>
-      <c r="I7" s="70"/>
+      <c r="I7" s="71"/>
       <c r="J7" s="42" t="s">
         <v>107</v>
       </c>
@@ -6394,8 +6403,8 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="70"/>
-      <c r="B8" s="71"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="15" t="s">
         <v>48</v>
       </c>
@@ -6411,7 +6420,7 @@
       <c r="G8" s="2">
         <v>14</v>
       </c>
-      <c r="I8" s="70"/>
+      <c r="I8" s="71"/>
       <c r="J8" s="42" t="s">
         <v>48</v>
       </c>
@@ -6429,8 +6438,8 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="70"/>
-      <c r="B9" s="71"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -6446,11 +6455,11 @@
       <c r="G9" s="2">
         <v>12</v>
       </c>
-      <c r="I9" s="70"/>
+      <c r="I9" s="71"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="70"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="9" t="s">
         <v>97</v>
       </c>
@@ -6466,21 +6475,21 @@
       <c r="G10" s="23">
         <v>12</v>
       </c>
-      <c r="I10" s="70"/>
+      <c r="I10" s="71"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="70"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="I11" s="70"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="70"/>
-      <c r="B12" s="74" t="s">
+      <c r="A12" s="71"/>
+      <c r="B12" s="75" t="s">
         <v>117</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -6498,7 +6507,7 @@
       <c r="G12" s="2">
         <v>14</v>
       </c>
-      <c r="I12" s="70"/>
+      <c r="I12" s="71"/>
       <c r="J12" s="39" t="s">
         <v>21</v>
       </c>
@@ -6516,8 +6525,8 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="70"/>
-      <c r="B13" s="74"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="15" t="s">
         <v>48</v>
       </c>
@@ -6533,7 +6542,7 @@
       <c r="G13" s="2">
         <v>14</v>
       </c>
-      <c r="I13" s="70"/>
+      <c r="I13" s="71"/>
       <c r="J13" s="42" t="s">
         <v>48</v>
       </c>
@@ -6551,8 +6560,8 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="70"/>
-      <c r="B14" s="74"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
@@ -6568,7 +6577,7 @@
       <c r="G14" s="23">
         <v>12</v>
       </c>
-      <c r="I14" s="70"/>
+      <c r="I14" s="71"/>
       <c r="J14" s="39"/>
       <c r="K14" s="21"/>
       <c r="L14" s="22"/>
@@ -6576,8 +6585,8 @@
       <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="70"/>
-      <c r="B15" s="75"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="76"/>
       <c r="C15" s="9" t="s">
         <v>97</v>
       </c>
@@ -6593,7 +6602,7 @@
       <c r="G15" s="23">
         <v>12</v>
       </c>
-      <c r="I15" s="70"/>
+      <c r="I15" s="71"/>
       <c r="J15" s="39" t="s">
         <v>97</v>
       </c>
@@ -6611,18 +6620,18 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="70"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="I16" s="70"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="I16" s="71"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="70"/>
-      <c r="B17" s="58" t="s">
+      <c r="A17" s="71"/>
+      <c r="B17" s="69" t="s">
         <v>113</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -6640,11 +6649,11 @@
       <c r="G17" s="23">
         <v>14</v>
       </c>
-      <c r="I17" s="70"/>
+      <c r="I17" s="71"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="70"/>
-      <c r="B18" s="74"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="8" t="s">
         <v>25</v>
       </c>
@@ -6660,11 +6669,11 @@
       <c r="G18" s="23">
         <v>13</v>
       </c>
-      <c r="I18" s="70"/>
+      <c r="I18" s="71"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="70"/>
-      <c r="B19" s="74"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="9" t="s">
         <v>21</v>
       </c>
@@ -6680,7 +6689,7 @@
       <c r="G19" s="23">
         <v>14</v>
       </c>
-      <c r="I19" s="70"/>
+      <c r="I19" s="71"/>
       <c r="J19" s="39" t="s">
         <v>21</v>
       </c>
@@ -6698,8 +6707,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="70"/>
-      <c r="B20" s="74"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="75"/>
       <c r="C20" s="15" t="s">
         <v>48</v>
       </c>
@@ -6715,7 +6724,7 @@
       <c r="G20" s="2">
         <v>14</v>
       </c>
-      <c r="I20" s="70"/>
+      <c r="I20" s="71"/>
       <c r="J20" s="42" t="s">
         <v>48</v>
       </c>
@@ -6733,8 +6742,8 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="70"/>
-      <c r="B21" s="74"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="9" t="s">
         <v>16</v>
       </c>
@@ -6750,7 +6759,7 @@
       <c r="G21" s="23">
         <v>12</v>
       </c>
-      <c r="I21" s="70"/>
+      <c r="I21" s="71"/>
       <c r="J21" s="39"/>
       <c r="K21" s="21"/>
       <c r="L21" s="22"/>
@@ -6758,8 +6767,8 @@
       <c r="N21" s="23"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="70"/>
-      <c r="B22" s="75"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="76"/>
       <c r="C22" s="9" t="s">
         <v>97</v>
       </c>
@@ -6775,7 +6784,7 @@
       <c r="G22" s="23">
         <v>12</v>
       </c>
-      <c r="I22" s="70"/>
+      <c r="I22" s="71"/>
       <c r="J22" s="39" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
W322 H1330 - Account (lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -2242,7 +2242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="126">
   <si>
     <t>2441268-0053441</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -2858,10 +2858,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Applied</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">301-168-120397       </t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -2870,7 +2866,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>W322 H1000</t>
+    <t>W322 H1530</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3156,7 +3152,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3236,11 +3232,42 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3260,49 +3287,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3669,7 +3662,7 @@
         <v>47</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -3677,58 +3670,58 @@
       <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:38" ht="16.399999999999999">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="48" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="I3" s="64" t="s">
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="I3" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
       <c r="Q3" s="28"/>
-      <c r="R3" s="49" t="s">
+      <c r="R3" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
       <c r="X3" s="33"/>
-      <c r="Y3" s="50" t="s">
+      <c r="Y3" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="51"/>
-      <c r="AE3" s="52"/>
+      <c r="Z3" s="62"/>
+      <c r="AA3" s="62"/>
+      <c r="AB3" s="62"/>
+      <c r="AC3" s="62"/>
+      <c r="AD3" s="62"/>
+      <c r="AE3" s="63"/>
       <c r="AF3" s="33"/>
-      <c r="AG3" s="50" t="s">
+      <c r="AG3" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="52"/>
+      <c r="AH3" s="62"/>
+      <c r="AI3" s="62"/>
+      <c r="AJ3" s="62"/>
+      <c r="AK3" s="62"/>
+      <c r="AL3" s="63"/>
     </row>
     <row r="4" spans="1:38" ht="16.399999999999999">
-      <c r="A4" s="55"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="11" t="s">
         <v>44</v>
       </c>
@@ -3833,19 +3826,19 @@
       </c>
     </row>
     <row r="5" spans="1:38">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
     </row>
     <row r="6" spans="1:38" ht="16.399999999999999">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="55" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -3871,8 +3864,8 @@
       <c r="O6" s="30"/>
     </row>
     <row r="7" spans="1:38" ht="16.399999999999999">
-      <c r="A7" s="60"/>
-      <c r="B7" s="63"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="9" t="s">
         <v>32</v>
       </c>
@@ -3894,58 +3887,32 @@
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="47" t="s">
-        <v>123</v>
-      </c>
+      <c r="N7" s="30"/>
       <c r="O7" s="30"/>
-      <c r="P7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="R7" s="47" t="s">
-        <v>123</v>
-      </c>
+      <c r="P7" s="30"/>
+      <c r="R7" s="30"/>
       <c r="T7" s="38" t="s">
         <v>108</v>
       </c>
       <c r="U7" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="V7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="W7" s="47" t="s">
-        <v>123</v>
-      </c>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
       <c r="Y7" s="30"/>
-      <c r="AB7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="AE7" s="47" t="s">
-        <v>123</v>
-      </c>
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="30"/>
+      <c r="AE7" s="30"/>
       <c r="AG7" s="30"/>
-      <c r="AI7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="AK7" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="AL7" s="47" t="s">
-        <v>123</v>
-      </c>
+      <c r="AI7" s="30"/>
+      <c r="AJ7" s="30"/>
+      <c r="AK7" s="30"/>
+      <c r="AL7" s="30"/>
     </row>
     <row r="8" spans="1:38" ht="16.399999999999999">
-      <c r="A8" s="60"/>
-      <c r="B8" s="63"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
@@ -3963,8 +3930,8 @@
       </c>
     </row>
     <row r="9" spans="1:38" ht="16.399999999999999">
-      <c r="A9" s="60"/>
-      <c r="B9" s="63"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
@@ -3982,8 +3949,8 @@
       </c>
     </row>
     <row r="10" spans="1:38" ht="16.399999999999999">
-      <c r="A10" s="60"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
@@ -4033,8 +4000,8 @@
       </c>
     </row>
     <row r="11" spans="1:38" ht="16.399999999999999">
-      <c r="A11" s="60"/>
-      <c r="B11" s="63"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
@@ -4084,8 +4051,8 @@
       </c>
     </row>
     <row r="12" spans="1:38" ht="16.399999999999999">
-      <c r="A12" s="60"/>
-      <c r="B12" s="63"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
@@ -4127,8 +4094,8 @@
       <c r="AL12" s="30"/>
     </row>
     <row r="13" spans="1:38" ht="16.399999999999999">
-      <c r="A13" s="61"/>
-      <c r="B13" s="63"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="9" t="s">
         <v>97</v>
       </c>
@@ -4170,23 +4137,23 @@
       <c r="AL13" s="30"/>
     </row>
     <row r="14" spans="1:38">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
       <c r="P14" s="37"/>
       <c r="W14" s="37"/>
       <c r="AE14" s="37"/>
       <c r="AL14" s="37"/>
     </row>
     <row r="15" spans="1:38" ht="16.399999999999999">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="55" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -4199,7 +4166,7 @@
         <v>120</v>
       </c>
       <c r="F15" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G15" s="2">
         <v>12</v>
@@ -4237,8 +4204,8 @@
       <c r="AL15" s="30"/>
     </row>
     <row r="16" spans="1:38" ht="16.399999999999999">
-      <c r="A16" s="60"/>
-      <c r="B16" s="63"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="6" t="s">
         <v>54</v>
       </c>
@@ -4260,8 +4227,8 @@
       <c r="AL16" s="37"/>
     </row>
     <row r="17" spans="1:38" ht="16.399999999999999">
-      <c r="A17" s="60"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="15" t="s">
         <v>107</v>
       </c>
@@ -4327,8 +4294,8 @@
       </c>
     </row>
     <row r="18" spans="1:38" ht="16.399999999999999">
-      <c r="A18" s="60"/>
-      <c r="B18" s="63"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="15" t="s">
         <v>48</v>
       </c>
@@ -4400,8 +4367,8 @@
       </c>
     </row>
     <row r="19" spans="1:38" ht="16.399999999999999">
-      <c r="A19" s="60"/>
-      <c r="B19" s="63"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
@@ -4460,8 +4427,8 @@
       </c>
     </row>
     <row r="20" spans="1:38" ht="16.399999999999999">
-      <c r="A20" s="61"/>
-      <c r="B20" s="63"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="9" t="s">
         <v>97</v>
       </c>
@@ -4520,23 +4487,23 @@
       </c>
     </row>
     <row r="21" spans="1:38">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
       <c r="P21" s="37"/>
       <c r="W21" s="37"/>
       <c r="AE21" s="37"/>
       <c r="AL21" s="37"/>
     </row>
     <row r="22" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="49" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -4559,8 +4526,8 @@
       <c r="AL22" s="37"/>
     </row>
     <row r="23" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A23" s="69"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="15" t="s">
         <v>54</v>
       </c>
@@ -4580,8 +4547,8 @@
       <c r="W23" s="37"/>
     </row>
     <row r="24" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A24" s="69"/>
-      <c r="B24" s="65"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="26" t="s">
         <v>73</v>
       </c>
@@ -4601,8 +4568,8 @@
       <c r="W24" s="37"/>
     </row>
     <row r="25" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A25" s="69"/>
-      <c r="B25" s="65"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="8" t="s">
         <v>25</v>
       </c>
@@ -4622,8 +4589,8 @@
       <c r="W25" s="37"/>
     </row>
     <row r="26" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A26" s="69"/>
-      <c r="B26" s="65"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="27" t="s">
         <v>76</v>
       </c>
@@ -4642,8 +4609,8 @@
       <c r="P26" s="37"/>
     </row>
     <row r="27" spans="1:38" ht="16.399999999999999">
-      <c r="A27" s="69"/>
-      <c r="B27" s="65"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="8" t="s">
         <v>64</v>
       </c>
@@ -4673,8 +4640,8 @@
       </c>
     </row>
     <row r="28" spans="1:38" ht="16.399999999999999">
-      <c r="A28" s="69"/>
-      <c r="B28" s="65"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
@@ -4704,8 +4671,8 @@
       </c>
     </row>
     <row r="29" spans="1:38" ht="16.399999999999999">
-      <c r="A29" s="69"/>
-      <c r="B29" s="65"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="8" t="s">
         <v>16</v>
       </c>
@@ -4724,8 +4691,8 @@
       <c r="P29" s="37"/>
     </row>
     <row r="30" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A30" s="70"/>
-      <c r="B30" s="65"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="9" t="s">
         <v>97</v>
       </c>
@@ -4744,20 +4711,20 @@
       <c r="P30" s="37"/>
     </row>
     <row r="31" spans="1:38" ht="16.399999999999999">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
       <c r="P31" s="37"/>
     </row>
     <row r="32" spans="1:38" ht="16.399999999999999">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="49" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -4778,8 +4745,8 @@
       <c r="P32" s="37"/>
     </row>
     <row r="33" spans="1:38" ht="16.399999999999999">
-      <c r="A33" s="55"/>
-      <c r="B33" s="65"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="8" t="s">
         <v>85</v>
       </c>
@@ -4800,8 +4767,8 @@
       <c r="AK33" s="30"/>
     </row>
     <row r="34" spans="1:38" ht="16.399999999999999">
-      <c r="A34" s="55"/>
-      <c r="B34" s="65"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="8" t="s">
         <v>64</v>
       </c>
@@ -4832,8 +4799,8 @@
       <c r="AK34" s="30"/>
     </row>
     <row r="35" spans="1:38" ht="16.399999999999999">
-      <c r="A35" s="55"/>
-      <c r="B35" s="65"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="15" t="s">
         <v>48</v>
       </c>
@@ -4852,8 +4819,8 @@
       <c r="P35" s="37"/>
     </row>
     <row r="36" spans="1:38" ht="16.399999999999999">
-      <c r="A36" s="55"/>
-      <c r="B36" s="65"/>
+      <c r="A36" s="48"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="8" t="s">
         <v>16</v>
       </c>
@@ -4877,8 +4844,8 @@
       <c r="AL36" s="30"/>
     </row>
     <row r="37" spans="1:38" ht="16.399999999999999">
-      <c r="A37" s="55"/>
-      <c r="B37" s="65"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="49"/>
       <c r="C37" s="9" t="s">
         <v>97</v>
       </c>
@@ -4934,14 +4901,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:B30"/>
     <mergeCell ref="R3:W3"/>
     <mergeCell ref="Y3:AE3"/>
     <mergeCell ref="AG3:AL3"/>
@@ -4952,6 +4911,14 @@
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="I3:P3"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4996,10 +4963,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="71" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -5017,7 +4984,7 @@
       <c r="G2" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="70" t="s">
         <v>93</v>
       </c>
       <c r="J2" s="39" t="s">
@@ -5037,8 +5004,8 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="71"/>
-      <c r="B3" s="72"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
@@ -5054,7 +5021,7 @@
       <c r="G3" s="2">
         <v>14</v>
       </c>
-      <c r="I3" s="71"/>
+      <c r="I3" s="70"/>
       <c r="J3" s="40" t="s">
         <v>19</v>
       </c>
@@ -5072,8 +5039,8 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -5089,11 +5056,11 @@
       <c r="G4" s="2">
         <v>12</v>
       </c>
-      <c r="I4" s="71"/>
+      <c r="I4" s="70"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="9" t="s">
         <v>97</v>
       </c>
@@ -5109,21 +5076,21 @@
       <c r="G5" s="23">
         <v>12</v>
       </c>
-      <c r="I5" s="71"/>
+      <c r="I5" s="70"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="71"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="I6" s="71"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="I6" s="70"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="71"/>
-      <c r="B7" s="72" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="71" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -5135,13 +5102,13 @@
       <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="48" t="s">
-        <v>125</v>
+      <c r="F7" s="47" t="s">
+        <v>124</v>
       </c>
       <c r="G7" s="2">
         <v>12</v>
       </c>
-      <c r="I7" s="71"/>
+      <c r="I7" s="70"/>
       <c r="J7" s="41" t="s">
         <v>11</v>
       </c>
@@ -5151,16 +5118,16 @@
       <c r="L7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="48" t="s">
-        <v>125</v>
+      <c r="M7" s="47" t="s">
+        <v>124</v>
       </c>
       <c r="N7" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="71"/>
-      <c r="B8" s="72"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="6" t="s">
         <v>54</v>
       </c>
@@ -5176,7 +5143,7 @@
       <c r="G8" s="2">
         <v>14</v>
       </c>
-      <c r="I8" s="71"/>
+      <c r="I8" s="70"/>
       <c r="J8" s="41" t="s">
         <v>54</v>
       </c>
@@ -5194,8 +5161,8 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="71"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="15" t="s">
         <v>107</v>
       </c>
@@ -5205,7 +5172,7 @@
       <c r="G9" s="2">
         <v>14</v>
       </c>
-      <c r="I9" s="71"/>
+      <c r="I9" s="70"/>
       <c r="J9" s="42" t="s">
         <v>107</v>
       </c>
@@ -5217,8 +5184,8 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="15" t="s">
         <v>48</v>
       </c>
@@ -5234,7 +5201,7 @@
       <c r="G10" s="2">
         <v>14</v>
       </c>
-      <c r="I10" s="71"/>
+      <c r="I10" s="70"/>
       <c r="J10" s="42" t="s">
         <v>48</v>
       </c>
@@ -5252,8 +5219,8 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="71"/>
-      <c r="B11" s="72"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="8" t="s">
         <v>16</v>
       </c>
@@ -5269,11 +5236,11 @@
       <c r="G11" s="2">
         <v>12</v>
       </c>
-      <c r="I11" s="71"/>
+      <c r="I11" s="70"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="71"/>
-      <c r="B12" s="72"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="9" t="s">
         <v>97</v>
       </c>
@@ -5289,21 +5256,21 @@
       <c r="G12" s="23">
         <v>12</v>
       </c>
-      <c r="I12" s="71"/>
+      <c r="I12" s="70"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="71"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="I13" s="71"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="I13" s="70"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="71"/>
-      <c r="B14" s="72" t="s">
+      <c r="A14" s="70"/>
+      <c r="B14" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -5321,7 +5288,7 @@
       <c r="G14" s="2">
         <v>14</v>
       </c>
-      <c r="I14" s="71"/>
+      <c r="I14" s="70"/>
       <c r="J14" s="39" t="s">
         <v>21</v>
       </c>
@@ -5339,8 +5306,8 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="71"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="15" t="s">
         <v>48</v>
       </c>
@@ -5356,7 +5323,7 @@
       <c r="G15" s="2">
         <v>14</v>
       </c>
-      <c r="I15" s="71"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="42" t="s">
         <v>48</v>
       </c>
@@ -5374,8 +5341,8 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="71"/>
-      <c r="B16" s="72"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="9" t="s">
         <v>16</v>
       </c>
@@ -5391,7 +5358,7 @@
       <c r="G16" s="23">
         <v>12</v>
       </c>
-      <c r="I16" s="71"/>
+      <c r="I16" s="70"/>
       <c r="J16" s="39"/>
       <c r="K16" s="21"/>
       <c r="L16" s="22"/>
@@ -5399,8 +5366,8 @@
       <c r="N16" s="23"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="71"/>
-      <c r="B17" s="72"/>
+      <c r="A17" s="70"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="9" t="s">
         <v>97</v>
       </c>
@@ -5416,7 +5383,7 @@
       <c r="G17" s="23">
         <v>12</v>
       </c>
-      <c r="I17" s="71"/>
+      <c r="I17" s="70"/>
       <c r="J17" s="39" t="s">
         <v>97</v>
       </c>
@@ -5434,18 +5401,18 @@
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="71"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="I18" s="71"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="I18" s="70"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="71"/>
-      <c r="B19" s="72" t="s">
+      <c r="A19" s="70"/>
+      <c r="B19" s="71" t="s">
         <v>113</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -5463,7 +5430,7 @@
       <c r="G19" s="23">
         <v>14</v>
       </c>
-      <c r="I19" s="71"/>
+      <c r="I19" s="70"/>
       <c r="J19" s="39" t="s">
         <v>21</v>
       </c>
@@ -5481,8 +5448,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72"/>
+      <c r="A20" s="70"/>
+      <c r="B20" s="71"/>
       <c r="C20" s="15" t="s">
         <v>48</v>
       </c>
@@ -5498,7 +5465,7 @@
       <c r="G20" s="2">
         <v>14</v>
       </c>
-      <c r="I20" s="71"/>
+      <c r="I20" s="70"/>
       <c r="J20" s="42" t="s">
         <v>48</v>
       </c>
@@ -5516,8 +5483,8 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="71"/>
-      <c r="B21" s="72"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="9" t="s">
         <v>16</v>
       </c>
@@ -5533,7 +5500,7 @@
       <c r="G21" s="23">
         <v>12</v>
       </c>
-      <c r="I21" s="71"/>
+      <c r="I21" s="70"/>
       <c r="J21" s="39"/>
       <c r="K21" s="21"/>
       <c r="L21" s="22"/>
@@ -5541,8 +5508,8 @@
       <c r="N21" s="23"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="71"/>
-      <c r="B22" s="72"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="9" t="s">
         <v>97</v>
       </c>
@@ -5558,7 +5525,7 @@
       <c r="G22" s="23">
         <v>12</v>
       </c>
-      <c r="I22" s="71"/>
+      <c r="I22" s="70"/>
       <c r="J22" s="39" t="s">
         <v>97</v>
       </c>
@@ -5614,7 +5581,7 @@
   <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.399999999999999"/>
@@ -5628,10 +5595,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="71" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -5649,7 +5616,7 @@
       <c r="G2" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="70" t="s">
         <v>93</v>
       </c>
       <c r="J2" s="39" t="s">
@@ -5669,8 +5636,8 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="71"/>
-      <c r="B3" s="72"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
@@ -5686,7 +5653,7 @@
       <c r="G3" s="2">
         <v>14</v>
       </c>
-      <c r="I3" s="71"/>
+      <c r="I3" s="70"/>
       <c r="J3" s="40" t="s">
         <v>19</v>
       </c>
@@ -5704,8 +5671,8 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -5721,11 +5688,11 @@
       <c r="G4" s="2">
         <v>12</v>
       </c>
-      <c r="I4" s="71"/>
+      <c r="I4" s="70"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="9" t="s">
         <v>97</v>
       </c>
@@ -5741,21 +5708,21 @@
       <c r="G5" s="23">
         <v>12</v>
       </c>
-      <c r="I5" s="71"/>
+      <c r="I5" s="70"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="71"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="I6" s="71"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="I6" s="70"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="71"/>
-      <c r="B7" s="72" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="71" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -5767,7 +5734,7 @@
       <c r="G7" s="2">
         <v>14</v>
       </c>
-      <c r="I7" s="71"/>
+      <c r="I7" s="70"/>
       <c r="J7" s="42" t="s">
         <v>107</v>
       </c>
@@ -5779,8 +5746,8 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="71"/>
-      <c r="B8" s="72"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="15" t="s">
         <v>48</v>
       </c>
@@ -5796,7 +5763,7 @@
       <c r="G8" s="2">
         <v>14</v>
       </c>
-      <c r="I8" s="71"/>
+      <c r="I8" s="70"/>
       <c r="J8" s="42" t="s">
         <v>48</v>
       </c>
@@ -5814,8 +5781,8 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="71"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -5831,11 +5798,11 @@
       <c r="G9" s="2">
         <v>12</v>
       </c>
-      <c r="I9" s="71"/>
+      <c r="I9" s="70"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="9" t="s">
         <v>97</v>
       </c>
@@ -5851,21 +5818,21 @@
       <c r="G10" s="23">
         <v>12</v>
       </c>
-      <c r="I10" s="71"/>
+      <c r="I10" s="70"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="71"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="I11" s="71"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="I11" s="70"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="71"/>
-      <c r="B12" s="68" t="s">
+      <c r="A12" s="70"/>
+      <c r="B12" s="57" t="s">
         <v>114</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -5883,11 +5850,11 @@
       <c r="G12" s="23">
         <v>14</v>
       </c>
-      <c r="I12" s="71"/>
+      <c r="I12" s="70"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="71"/>
-      <c r="B13" s="75"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="15" t="s">
         <v>54</v>
       </c>
@@ -5903,11 +5870,11 @@
       <c r="G13" s="2">
         <v>14</v>
       </c>
-      <c r="I13" s="71"/>
+      <c r="I13" s="70"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="71"/>
-      <c r="B14" s="75"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
@@ -5923,11 +5890,11 @@
       <c r="G14" s="2">
         <v>13</v>
       </c>
-      <c r="I14" s="71"/>
+      <c r="I14" s="70"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="71"/>
-      <c r="B15" s="75"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="9" t="s">
         <v>21</v>
       </c>
@@ -5943,7 +5910,7 @@
       <c r="G15" s="2">
         <v>14</v>
       </c>
-      <c r="I15" s="71"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="39" t="s">
         <v>21</v>
       </c>
@@ -5961,8 +5928,8 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="71"/>
-      <c r="B16" s="75"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="15" t="s">
         <v>48</v>
       </c>
@@ -5978,7 +5945,7 @@
       <c r="G16" s="2">
         <v>14</v>
       </c>
-      <c r="I16" s="71"/>
+      <c r="I16" s="70"/>
       <c r="J16" s="42" t="s">
         <v>48</v>
       </c>
@@ -5996,8 +5963,8 @@
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="71"/>
-      <c r="B17" s="75"/>
+      <c r="A17" s="70"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
@@ -6013,7 +5980,7 @@
       <c r="G17" s="23">
         <v>12</v>
       </c>
-      <c r="I17" s="71"/>
+      <c r="I17" s="70"/>
       <c r="J17" s="39"/>
       <c r="K17" s="21"/>
       <c r="L17" s="22"/>
@@ -6021,8 +5988,8 @@
       <c r="N17" s="23"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="71"/>
-      <c r="B18" s="76"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="9" t="s">
         <v>97</v>
       </c>
@@ -6038,7 +6005,7 @@
       <c r="G18" s="23">
         <v>12</v>
       </c>
-      <c r="I18" s="71"/>
+      <c r="I18" s="70"/>
       <c r="J18" s="39" t="s">
         <v>97</v>
       </c>
@@ -6056,18 +6023,18 @@
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="71"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="I19" s="71"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="72"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="I19" s="70"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72" t="s">
+      <c r="A20" s="70"/>
+      <c r="B20" s="71" t="s">
         <v>113</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -6085,7 +6052,7 @@
       <c r="G20" s="23">
         <v>14</v>
       </c>
-      <c r="I20" s="71"/>
+      <c r="I20" s="70"/>
       <c r="J20" s="39" t="s">
         <v>21</v>
       </c>
@@ -6103,8 +6070,8 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="71"/>
-      <c r="B21" s="72"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="15" t="s">
         <v>48</v>
       </c>
@@ -6120,7 +6087,7 @@
       <c r="G21" s="2">
         <v>14</v>
       </c>
-      <c r="I21" s="71"/>
+      <c r="I21" s="70"/>
       <c r="J21" s="42" t="s">
         <v>48</v>
       </c>
@@ -6138,8 +6105,8 @@
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="71"/>
-      <c r="B22" s="72"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="9" t="s">
         <v>16</v>
       </c>
@@ -6155,7 +6122,7 @@
       <c r="G22" s="23">
         <v>12</v>
       </c>
-      <c r="I22" s="71"/>
+      <c r="I22" s="70"/>
       <c r="J22" s="39"/>
       <c r="K22" s="21"/>
       <c r="L22" s="22"/>
@@ -6163,8 +6130,8 @@
       <c r="N22" s="23"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="71"/>
-      <c r="B23" s="72"/>
+      <c r="A23" s="70"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="9" t="s">
         <v>97</v>
       </c>
@@ -6180,7 +6147,7 @@
       <c r="G23" s="23">
         <v>12</v>
       </c>
-      <c r="I23" s="71"/>
+      <c r="I23" s="70"/>
       <c r="J23" s="39" t="s">
         <v>97</v>
       </c>
@@ -6236,7 +6203,7 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B16" sqref="B16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.399999999999999"/>
@@ -6250,10 +6217,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="71" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -6271,7 +6238,7 @@
       <c r="G2" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="70" t="s">
         <v>93</v>
       </c>
       <c r="J2" s="39" t="s">
@@ -6291,8 +6258,8 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="71"/>
-      <c r="B3" s="72"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
@@ -6308,7 +6275,7 @@
       <c r="G3" s="2">
         <v>14</v>
       </c>
-      <c r="I3" s="71"/>
+      <c r="I3" s="70"/>
       <c r="J3" s="40" t="s">
         <v>19</v>
       </c>
@@ -6326,8 +6293,8 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="8" t="s">
         <v>16</v>
       </c>
@@ -6343,11 +6310,11 @@
       <c r="G4" s="2">
         <v>12</v>
       </c>
-      <c r="I4" s="71"/>
+      <c r="I4" s="70"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="9" t="s">
         <v>97</v>
       </c>
@@ -6363,23 +6330,23 @@
       <c r="G5" s="23">
         <v>12</v>
       </c>
-      <c r="I5" s="71"/>
+      <c r="I5" s="70"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="71"/>
-      <c r="B6" s="66" t="s">
+      <c r="A6" s="70"/>
+      <c r="B6" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="I6" s="71"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="I6" s="70"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="71"/>
-      <c r="B7" s="72" t="s">
+      <c r="A7" s="70"/>
+      <c r="B7" s="71" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -6391,7 +6358,7 @@
       <c r="G7" s="2">
         <v>14</v>
       </c>
-      <c r="I7" s="71"/>
+      <c r="I7" s="70"/>
       <c r="J7" s="42" t="s">
         <v>107</v>
       </c>
@@ -6403,8 +6370,8 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="71"/>
-      <c r="B8" s="72"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="15" t="s">
         <v>48</v>
       </c>
@@ -6420,7 +6387,7 @@
       <c r="G8" s="2">
         <v>14</v>
       </c>
-      <c r="I8" s="71"/>
+      <c r="I8" s="70"/>
       <c r="J8" s="42" t="s">
         <v>48</v>
       </c>
@@ -6438,8 +6405,8 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="71"/>
-      <c r="B9" s="72"/>
+      <c r="A9" s="70"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
@@ -6455,11 +6422,11 @@
       <c r="G9" s="2">
         <v>12</v>
       </c>
-      <c r="I9" s="71"/>
+      <c r="I9" s="70"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
+      <c r="A10" s="70"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="9" t="s">
         <v>97</v>
       </c>
@@ -6475,21 +6442,21 @@
       <c r="G10" s="23">
         <v>12</v>
       </c>
-      <c r="I10" s="71"/>
+      <c r="I10" s="70"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="71"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="I11" s="71"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="I11" s="70"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="71"/>
-      <c r="B12" s="75" t="s">
+      <c r="A12" s="70"/>
+      <c r="B12" s="74" t="s">
         <v>117</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -6507,7 +6474,7 @@
       <c r="G12" s="2">
         <v>14</v>
       </c>
-      <c r="I12" s="71"/>
+      <c r="I12" s="70"/>
       <c r="J12" s="39" t="s">
         <v>21</v>
       </c>
@@ -6525,8 +6492,8 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="71"/>
-      <c r="B13" s="75"/>
+      <c r="A13" s="70"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="15" t="s">
         <v>48</v>
       </c>
@@ -6542,7 +6509,7 @@
       <c r="G13" s="2">
         <v>14</v>
       </c>
-      <c r="I13" s="71"/>
+      <c r="I13" s="70"/>
       <c r="J13" s="42" t="s">
         <v>48</v>
       </c>
@@ -6560,8 +6527,8 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="71"/>
-      <c r="B14" s="75"/>
+      <c r="A14" s="70"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
@@ -6577,7 +6544,7 @@
       <c r="G14" s="23">
         <v>12</v>
       </c>
-      <c r="I14" s="71"/>
+      <c r="I14" s="70"/>
       <c r="J14" s="39"/>
       <c r="K14" s="21"/>
       <c r="L14" s="22"/>
@@ -6585,8 +6552,8 @@
       <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="71"/>
-      <c r="B15" s="76"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="9" t="s">
         <v>97</v>
       </c>
@@ -6602,7 +6569,7 @@
       <c r="G15" s="23">
         <v>12</v>
       </c>
-      <c r="I15" s="71"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="39" t="s">
         <v>97</v>
       </c>
@@ -6620,18 +6587,18 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="71"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="I16" s="71"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="I16" s="70"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="71"/>
-      <c r="B17" s="69" t="s">
+      <c r="A17" s="70"/>
+      <c r="B17" s="58" t="s">
         <v>113</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -6649,11 +6616,11 @@
       <c r="G17" s="23">
         <v>14</v>
       </c>
-      <c r="I17" s="71"/>
+      <c r="I17" s="70"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="71"/>
-      <c r="B18" s="75"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="8" t="s">
         <v>25</v>
       </c>
@@ -6669,11 +6636,11 @@
       <c r="G18" s="23">
         <v>13</v>
       </c>
-      <c r="I18" s="71"/>
+      <c r="I18" s="70"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="71"/>
-      <c r="B19" s="75"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="9" t="s">
         <v>21</v>
       </c>
@@ -6689,7 +6656,7 @@
       <c r="G19" s="23">
         <v>14</v>
       </c>
-      <c r="I19" s="71"/>
+      <c r="I19" s="70"/>
       <c r="J19" s="39" t="s">
         <v>21</v>
       </c>
@@ -6707,8 +6674,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="71"/>
-      <c r="B20" s="75"/>
+      <c r="A20" s="70"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="15" t="s">
         <v>48</v>
       </c>
@@ -6724,7 +6691,7 @@
       <c r="G20" s="2">
         <v>14</v>
       </c>
-      <c r="I20" s="71"/>
+      <c r="I20" s="70"/>
       <c r="J20" s="42" t="s">
         <v>48</v>
       </c>
@@ -6742,8 +6709,8 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="71"/>
-      <c r="B21" s="75"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="9" t="s">
         <v>16</v>
       </c>
@@ -6759,7 +6726,7 @@
       <c r="G21" s="23">
         <v>12</v>
       </c>
-      <c r="I21" s="71"/>
+      <c r="I21" s="70"/>
       <c r="J21" s="39"/>
       <c r="K21" s="21"/>
       <c r="L21" s="22"/>
@@ -6767,8 +6734,8 @@
       <c r="N21" s="23"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="71"/>
-      <c r="B22" s="76"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="9" t="s">
         <v>97</v>
       </c>
@@ -6784,7 +6751,7 @@
       <c r="G22" s="23">
         <v>12</v>
       </c>
-      <c r="I22" s="71"/>
+      <c r="I22" s="70"/>
       <c r="J22" s="39" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
W337 H1630-Account & Account(lite)
</commit_message>
<xml_diff>
--- a/Account-2019 (lite).xlsx
+++ b/Account-2019 (lite).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\共用\Github\Family\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="419" yWindow="105" windowWidth="16979" windowHeight="6336" tabRatio="508"/>
+    <workbookView xWindow="420" yWindow="110" windowWidth="16980" windowHeight="6340" tabRatio="508"/>
   </bookViews>
   <sheets>
     <sheet name="金融簡易版" sheetId="4" r:id="rId1"/>
@@ -22,7 +27,7 @@
     <author>Bali-ThinkPad</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -118,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -280,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -354,7 +359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R12" authorId="0">
+    <comment ref="R12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="0">
+    <comment ref="C15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -443,7 +448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0">
+    <comment ref="C19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -477,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0">
+    <comment ref="H19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -511,7 +516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C25" authorId="0">
+    <comment ref="C25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -546,7 +551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C29" authorId="0">
+    <comment ref="C29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -580,7 +585,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="0">
+    <comment ref="C33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -615,7 +620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C36" authorId="0">
+    <comment ref="C36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -659,7 +664,7 @@
     <author>Bali-ThinkPad</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -751,7 +756,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -843,7 +848,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -877,7 +882,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -911,7 +916,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -985,7 +990,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1019,7 +1024,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1053,7 +1058,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0">
+    <comment ref="J16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1087,7 +1092,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0">
+    <comment ref="C21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1121,7 +1126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J21" authorId="0">
+    <comment ref="J21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1165,7 +1170,7 @@
     <author>Bali-ThinkPad</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1257,7 +1262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1349,7 +1354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1383,7 +1388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1417,7 +1422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1491,7 +1496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1525,7 +1530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1560,7 +1565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1594,7 +1599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J17" authorId="0">
+    <comment ref="J17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1628,7 +1633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0">
+    <comment ref="C22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1662,7 +1667,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0">
+    <comment ref="J22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1706,7 +1711,7 @@
     <author>Bali-ThinkPad</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1798,7 +1803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1890,7 +1895,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1924,7 +1929,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1958,7 +1963,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2032,7 +2037,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2066,7 +2071,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2100,7 +2105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0">
+    <comment ref="J14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2134,7 +2139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0">
+    <comment ref="C18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2169,7 +2174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0">
+    <comment ref="C21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2203,7 +2208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J21" authorId="0">
+    <comment ref="J21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2870,15 +2875,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>W334 H1430</t>
+    <t>W337 H1630</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3240,6 +3245,40 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3258,49 +3297,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3382,7 +3387,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3414,9 +3419,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3448,6 +3454,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3623,44 +3630,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A2:AL42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.05" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.625" style="1" customWidth="1"/>
-    <col min="10" max="16" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.625" style="1" customWidth="1"/>
-    <col min="19" max="23" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="5.625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="10.625" style="1" customWidth="1"/>
-    <col min="26" max="31" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="5.625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="10.625" style="1" customWidth="1"/>
-    <col min="34" max="38" width="10.625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="16384" width="8.875" style="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="16.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.90625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.26953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.36328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" style="1" customWidth="1"/>
+    <col min="10" max="16" width="10.6328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="5.6328125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6328125" style="1" customWidth="1"/>
+    <col min="19" max="23" width="10.6328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="5.6328125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="10.6328125" style="1" customWidth="1"/>
+    <col min="26" max="31" width="10.6328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="5.6328125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="10.6328125" style="1" customWidth="1"/>
+    <col min="34" max="38" width="10.6328125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:38" ht="16.399999999999999">
+    <row r="2" spans="1:38" ht="17" x14ac:dyDescent="0.4">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14" t="s">
@@ -3674,59 +3681,59 @@
       <c r="G2" s="13"/>
       <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="1:38" ht="16.399999999999999">
-      <c r="A3" s="55" t="s">
+    <row r="3" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A3" s="49" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="I3" s="64" t="s">
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="I3" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
       <c r="Q3" s="28"/>
-      <c r="R3" s="49" t="s">
+      <c r="R3" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="49"/>
-      <c r="W3" s="49"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
       <c r="X3" s="33"/>
-      <c r="Y3" s="50" t="s">
+      <c r="Y3" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="51"/>
-      <c r="AE3" s="52"/>
+      <c r="Z3" s="63"/>
+      <c r="AA3" s="63"/>
+      <c r="AB3" s="63"/>
+      <c r="AC3" s="63"/>
+      <c r="AD3" s="63"/>
+      <c r="AE3" s="64"/>
       <c r="AF3" s="33"/>
-      <c r="AG3" s="50" t="s">
+      <c r="AG3" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="52"/>
-    </row>
-    <row r="4" spans="1:38" ht="16.399999999999999">
-      <c r="A4" s="55"/>
+      <c r="AH3" s="63"/>
+      <c r="AI3" s="63"/>
+      <c r="AJ3" s="63"/>
+      <c r="AK3" s="63"/>
+      <c r="AL3" s="64"/>
+    </row>
+    <row r="4" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A4" s="49"/>
       <c r="B4" s="11" t="s">
         <v>44</v>
       </c>
@@ -3830,20 +3837,20 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-    </row>
-    <row r="6" spans="1:38" ht="16.399999999999999">
-      <c r="A6" s="59" t="s">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A5" s="68"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+    </row>
+    <row r="6" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A6" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="56" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -3868,9 +3875,9 @@
       <c r="M6" s="30"/>
       <c r="O6" s="30"/>
     </row>
-    <row r="7" spans="1:38" ht="16.399999999999999">
-      <c r="A7" s="60"/>
-      <c r="B7" s="63"/>
+    <row r="7" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A7" s="54"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="9" t="s">
         <v>32</v>
       </c>
@@ -3915,9 +3922,9 @@
       <c r="AK7" s="30"/>
       <c r="AL7" s="30"/>
     </row>
-    <row r="8" spans="1:38" ht="16.399999999999999">
-      <c r="A8" s="60"/>
-      <c r="B8" s="63"/>
+    <row r="8" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A8" s="54"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
@@ -3934,9 +3941,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="16.399999999999999">
-      <c r="A9" s="60"/>
-      <c r="B9" s="63"/>
+    <row r="9" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A9" s="54"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
@@ -3953,9 +3960,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="16.399999999999999">
-      <c r="A10" s="60"/>
-      <c r="B10" s="63"/>
+    <row r="10" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A10" s="54"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
@@ -4004,9 +4011,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="16.399999999999999">
-      <c r="A11" s="60"/>
-      <c r="B11" s="63"/>
+    <row r="11" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A11" s="54"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
@@ -4055,9 +4062,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="16.399999999999999">
-      <c r="A12" s="60"/>
-      <c r="B12" s="63"/>
+    <row r="12" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A12" s="54"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
@@ -4098,9 +4105,9 @@
       <c r="AK12" s="30"/>
       <c r="AL12" s="30"/>
     </row>
-    <row r="13" spans="1:38" ht="16.399999999999999">
-      <c r="A13" s="61"/>
-      <c r="B13" s="63"/>
+    <row r="13" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A13" s="55"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="9" t="s">
         <v>97</v>
       </c>
@@ -4141,24 +4148,24 @@
       <c r="AK13" s="30"/>
       <c r="AL13" s="30"/>
     </row>
-    <row r="14" spans="1:38">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
       <c r="P14" s="37"/>
       <c r="W14" s="37"/>
       <c r="AE14" s="37"/>
       <c r="AL14" s="37"/>
     </row>
-    <row r="15" spans="1:38" ht="16.399999999999999">
-      <c r="A15" s="67" t="s">
+    <row r="15" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A15" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -4208,9 +4215,9 @@
       <c r="AK15" s="30"/>
       <c r="AL15" s="30"/>
     </row>
-    <row r="16" spans="1:38" ht="16.399999999999999">
-      <c r="A16" s="60"/>
-      <c r="B16" s="63"/>
+    <row r="16" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A16" s="54"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="6" t="s">
         <v>54</v>
       </c>
@@ -4231,9 +4238,9 @@
       <c r="AE16" s="37"/>
       <c r="AL16" s="37"/>
     </row>
-    <row r="17" spans="1:38" ht="16.399999999999999">
-      <c r="A17" s="60"/>
-      <c r="B17" s="63"/>
+    <row r="17" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A17" s="54"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="15" t="s">
         <v>107</v>
       </c>
@@ -4270,9 +4277,9 @@
       <c r="AK17" s="30"/>
       <c r="AL17" s="30"/>
     </row>
-    <row r="18" spans="1:38" ht="16.399999999999999">
-      <c r="A18" s="60"/>
-      <c r="B18" s="63"/>
+    <row r="18" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A18" s="54"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="15" t="s">
         <v>48</v>
       </c>
@@ -4309,9 +4316,9 @@
       <c r="AK18" s="30"/>
       <c r="AL18" s="30"/>
     </row>
-    <row r="19" spans="1:38" ht="16.399999999999999">
-      <c r="A19" s="60"/>
-      <c r="B19" s="63"/>
+    <row r="19" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A19" s="54"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="8" t="s">
         <v>16</v>
       </c>
@@ -4351,9 +4358,9 @@
       <c r="AK19" s="30"/>
       <c r="AL19" s="30"/>
     </row>
-    <row r="20" spans="1:38" ht="16.399999999999999">
-      <c r="A20" s="61"/>
-      <c r="B20" s="63"/>
+    <row r="20" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A20" s="55"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="9" t="s">
         <v>97</v>
       </c>
@@ -4393,24 +4400,24 @@
       <c r="AK20" s="30"/>
       <c r="AL20" s="30"/>
     </row>
-    <row r="21" spans="1:38">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="A21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
       <c r="P21" s="37"/>
       <c r="W21" s="37"/>
       <c r="AE21" s="37"/>
       <c r="AL21" s="37"/>
     </row>
-    <row r="22" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A22" s="68" t="s">
+    <row r="22" spans="1:38" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="50" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -4432,9 +4439,9 @@
       <c r="W22" s="37"/>
       <c r="AL22" s="37"/>
     </row>
-    <row r="23" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A23" s="69"/>
-      <c r="B23" s="65"/>
+    <row r="23" spans="1:38" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="59"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="15" t="s">
         <v>54</v>
       </c>
@@ -4453,9 +4460,9 @@
       <c r="P23" s="37"/>
       <c r="W23" s="37"/>
     </row>
-    <row r="24" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A24" s="69"/>
-      <c r="B24" s="65"/>
+    <row r="24" spans="1:38" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="59"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="26" t="s">
         <v>73</v>
       </c>
@@ -4474,9 +4481,9 @@
       <c r="P24" s="37"/>
       <c r="W24" s="37"/>
     </row>
-    <row r="25" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A25" s="69"/>
-      <c r="B25" s="65"/>
+    <row r="25" spans="1:38" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="59"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="8" t="s">
         <v>25</v>
       </c>
@@ -4495,9 +4502,9 @@
       <c r="P25" s="37"/>
       <c r="W25" s="37"/>
     </row>
-    <row r="26" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A26" s="69"/>
-      <c r="B26" s="65"/>
+    <row r="26" spans="1:38" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="59"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="27" t="s">
         <v>76</v>
       </c>
@@ -4515,9 +4522,9 @@
       </c>
       <c r="P26" s="37"/>
     </row>
-    <row r="27" spans="1:38" ht="16.399999999999999">
-      <c r="A27" s="69"/>
-      <c r="B27" s="65"/>
+    <row r="27" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A27" s="59"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="8" t="s">
         <v>64</v>
       </c>
@@ -4546,9 +4553,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:38" ht="16.399999999999999">
-      <c r="A28" s="69"/>
-      <c r="B28" s="65"/>
+    <row r="28" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A28" s="59"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
@@ -4577,9 +4584,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="16.399999999999999">
-      <c r="A29" s="69"/>
-      <c r="B29" s="65"/>
+    <row r="29" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A29" s="59"/>
+      <c r="B29" s="50"/>
       <c r="C29" s="8" t="s">
         <v>16</v>
       </c>
@@ -4597,9 +4604,9 @@
       </c>
       <c r="P29" s="37"/>
     </row>
-    <row r="30" spans="1:38" ht="16.399999999999999" customHeight="1">
-      <c r="A30" s="70"/>
-      <c r="B30" s="65"/>
+    <row r="30" spans="1:38" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="60"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="9" t="s">
         <v>97</v>
       </c>
@@ -4617,21 +4624,21 @@
       </c>
       <c r="P30" s="37"/>
     </row>
-    <row r="31" spans="1:38" ht="16.399999999999999">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
+    <row r="31" spans="1:38" ht="17" x14ac:dyDescent="0.35">
+      <c r="A31" s="65"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
       <c r="P31" s="37"/>
     </row>
-    <row r="32" spans="1:38" ht="16.399999999999999">
-      <c r="A32" s="55" t="s">
+    <row r="32" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A32" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="50" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -4651,9 +4658,9 @@
       </c>
       <c r="P32" s="37"/>
     </row>
-    <row r="33" spans="1:38" ht="16.399999999999999">
-      <c r="A33" s="55"/>
-      <c r="B33" s="65"/>
+    <row r="33" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A33" s="49"/>
+      <c r="B33" s="50"/>
       <c r="C33" s="8" t="s">
         <v>85</v>
       </c>
@@ -4673,9 +4680,9 @@
       <c r="P33" s="37"/>
       <c r="AK33" s="30"/>
     </row>
-    <row r="34" spans="1:38" ht="16.399999999999999">
-      <c r="A34" s="55"/>
-      <c r="B34" s="65"/>
+    <row r="34" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A34" s="49"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="8" t="s">
         <v>64</v>
       </c>
@@ -4694,7 +4701,7 @@
       <c r="M34" s="30"/>
       <c r="N34" s="30"/>
       <c r="O34" s="30"/>
-      <c r="P34" s="37"/>
+      <c r="P34" s="30"/>
       <c r="U34" s="30"/>
       <c r="V34" s="30"/>
       <c r="AB34" s="30"/>
@@ -4705,9 +4712,9 @@
       <c r="AJ34" s="30"/>
       <c r="AK34" s="30"/>
     </row>
-    <row r="35" spans="1:38" ht="16.399999999999999">
-      <c r="A35" s="55"/>
-      <c r="B35" s="65"/>
+    <row r="35" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A35" s="49"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="15" t="s">
         <v>48</v>
       </c>
@@ -4723,11 +4730,14 @@
       <c r="G35" s="2">
         <v>14</v>
       </c>
-      <c r="P35" s="37"/>
-    </row>
-    <row r="36" spans="1:38" ht="16.399999999999999">
-      <c r="A36" s="55"/>
-      <c r="B36" s="65"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="30"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="30"/>
+    </row>
+    <row r="36" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A36" s="49"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="8" t="s">
         <v>16</v>
       </c>
@@ -4743,6 +4753,8 @@
       <c r="G36" s="23">
         <v>12</v>
       </c>
+      <c r="M36" s="30"/>
+      <c r="N36" s="30"/>
       <c r="O36" s="30"/>
       <c r="P36" s="30"/>
       <c r="V36" s="30"/>
@@ -4750,9 +4762,9 @@
       <c r="AK36" s="30"/>
       <c r="AL36" s="30"/>
     </row>
-    <row r="37" spans="1:38" ht="16.399999999999999">
-      <c r="A37" s="55"/>
-      <c r="B37" s="65"/>
+    <row r="37" spans="1:38" ht="17" x14ac:dyDescent="0.4">
+      <c r="A37" s="49"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="9" t="s">
         <v>97</v>
       </c>
@@ -4768,6 +4780,8 @@
       <c r="G37" s="23">
         <v>12</v>
       </c>
+      <c r="M37" s="30"/>
+      <c r="N37" s="30"/>
       <c r="O37" s="30"/>
       <c r="P37" s="30"/>
       <c r="V37" s="30"/>
@@ -4775,7 +4789,7 @@
       <c r="AK37" s="30"/>
       <c r="AL37" s="30"/>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="17"/>
@@ -4785,7 +4799,7 @@
       <c r="G38" s="17"/>
       <c r="P38" s="37"/>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -4795,27 +4809,19 @@
       <c r="G39" s="17"/>
       <c r="P39" s="37"/>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="P40" s="37"/>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.35">
       <c r="P41" s="37"/>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.35">
       <c r="P42" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:B30"/>
     <mergeCell ref="R3:W3"/>
     <mergeCell ref="Y3:AE3"/>
     <mergeCell ref="AG3:AL3"/>
@@ -4826,6 +4832,14 @@
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="I3:P3"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4852,24 +4866,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="10" max="10" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="24.5" customWidth="1"/>
+    <col min="13" max="13" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="71" t="s">
         <v>109</v>
       </c>
@@ -4910,7 +4924,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="71"/>
       <c r="B3" s="72"/>
       <c r="C3" s="8" t="s">
@@ -4945,7 +4959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="71"/>
       <c r="B4" s="72"/>
       <c r="C4" s="8" t="s">
@@ -4965,7 +4979,7 @@
       </c>
       <c r="I4" s="71"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="71"/>
       <c r="B5" s="72"/>
       <c r="C5" s="9" t="s">
@@ -4985,17 +4999,17 @@
       </c>
       <c r="I5" s="71"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="71"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
       <c r="I6" s="71"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="71"/>
       <c r="B7" s="72" t="s">
         <v>13</v>
@@ -5032,7 +5046,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="71"/>
       <c r="B8" s="72"/>
       <c r="C8" s="6" t="s">
@@ -5067,7 +5081,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="71"/>
       <c r="B9" s="72"/>
       <c r="C9" s="15" t="s">
@@ -5090,7 +5104,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="71"/>
       <c r="B10" s="72"/>
       <c r="C10" s="15" t="s">
@@ -5125,7 +5139,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="71"/>
       <c r="B11" s="72"/>
       <c r="C11" s="8" t="s">
@@ -5145,7 +5159,7 @@
       </c>
       <c r="I11" s="71"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="71"/>
       <c r="B12" s="72"/>
       <c r="C12" s="9" t="s">
@@ -5165,17 +5179,17 @@
       </c>
       <c r="I12" s="71"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="71"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
       <c r="I13" s="71"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="71"/>
       <c r="B14" s="72" t="s">
         <v>114</v>
@@ -5212,7 +5226,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="71"/>
       <c r="B15" s="72"/>
       <c r="C15" s="15" t="s">
@@ -5247,7 +5261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="71"/>
       <c r="B16" s="72"/>
       <c r="C16" s="9" t="s">
@@ -5272,7 +5286,7 @@
       <c r="M16" s="22"/>
       <c r="N16" s="23"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="71"/>
       <c r="B17" s="72"/>
       <c r="C17" s="9" t="s">
@@ -5307,7 +5321,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" s="71"/>
       <c r="B18" s="73"/>
       <c r="C18" s="74"/>
@@ -5317,7 +5331,7 @@
       <c r="G18" s="74"/>
       <c r="I18" s="71"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="71"/>
       <c r="B19" s="72" t="s">
         <v>113</v>
@@ -5354,7 +5368,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" s="71"/>
       <c r="B20" s="72"/>
       <c r="C20" s="15" t="s">
@@ -5389,7 +5403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21" s="71"/>
       <c r="B21" s="72"/>
       <c r="C21" s="9" t="s">
@@ -5414,7 +5428,7 @@
       <c r="M21" s="22"/>
       <c r="N21" s="23"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22" s="71"/>
       <c r="B22" s="72"/>
       <c r="C22" s="9" t="s">
@@ -5484,24 +5498,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="10" max="10" width="15.25" customWidth="1"/>
-    <col min="12" max="12" width="10.75" customWidth="1"/>
-    <col min="13" max="13" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" customWidth="1"/>
+    <col min="13" max="13" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="71" t="s">
         <v>109</v>
       </c>
@@ -5542,7 +5556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="71"/>
       <c r="B3" s="72"/>
       <c r="C3" s="8" t="s">
@@ -5577,7 +5591,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="71"/>
       <c r="B4" s="72"/>
       <c r="C4" s="8" t="s">
@@ -5597,7 +5611,7 @@
       </c>
       <c r="I4" s="71"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="71"/>
       <c r="B5" s="72"/>
       <c r="C5" s="9" t="s">
@@ -5617,17 +5631,17 @@
       </c>
       <c r="I5" s="71"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="71"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
       <c r="I6" s="71"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="71"/>
       <c r="B7" s="72" t="s">
         <v>115</v>
@@ -5652,7 +5666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="71"/>
       <c r="B8" s="72"/>
       <c r="C8" s="15" t="s">
@@ -5687,7 +5701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="71"/>
       <c r="B9" s="72"/>
       <c r="C9" s="8" t="s">
@@ -5707,7 +5721,7 @@
       </c>
       <c r="I9" s="71"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="71"/>
       <c r="B10" s="72"/>
       <c r="C10" s="9" t="s">
@@ -5727,19 +5741,19 @@
       </c>
       <c r="I10" s="71"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="71"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
       <c r="I11" s="71"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="71"/>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="58" t="s">
         <v>114</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -5759,7 +5773,7 @@
       </c>
       <c r="I12" s="71"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="71"/>
       <c r="B13" s="75"/>
       <c r="C13" s="15" t="s">
@@ -5779,7 +5793,7 @@
       </c>
       <c r="I13" s="71"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="71"/>
       <c r="B14" s="75"/>
       <c r="C14" s="8" t="s">
@@ -5799,7 +5813,7 @@
       </c>
       <c r="I14" s="71"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="71"/>
       <c r="B15" s="75"/>
       <c r="C15" s="9" t="s">
@@ -5834,7 +5848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="71"/>
       <c r="B16" s="75"/>
       <c r="C16" s="15" t="s">
@@ -5869,7 +5883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="71"/>
       <c r="B17" s="75"/>
       <c r="C17" s="9" t="s">
@@ -5894,7 +5908,7 @@
       <c r="M17" s="22"/>
       <c r="N17" s="23"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" s="71"/>
       <c r="B18" s="76"/>
       <c r="C18" s="9" t="s">
@@ -5929,7 +5943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="71"/>
       <c r="B19" s="73"/>
       <c r="C19" s="74"/>
@@ -5939,7 +5953,7 @@
       <c r="G19" s="74"/>
       <c r="I19" s="71"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" s="71"/>
       <c r="B20" s="72" t="s">
         <v>113</v>
@@ -5976,7 +5990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21" s="71"/>
       <c r="B21" s="72"/>
       <c r="C21" s="15" t="s">
@@ -6011,7 +6025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22" s="71"/>
       <c r="B22" s="72"/>
       <c r="C22" s="9" t="s">
@@ -6036,7 +6050,7 @@
       <c r="M22" s="22"/>
       <c r="N22" s="23"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A23" s="71"/>
       <c r="B23" s="72"/>
       <c r="C23" s="9" t="s">
@@ -6106,24 +6120,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="10" max="10" width="15.25" customWidth="1"/>
-    <col min="12" max="12" width="10.75" customWidth="1"/>
-    <col min="13" max="13" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" customWidth="1"/>
+    <col min="13" max="13" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="71" t="s">
         <v>109</v>
       </c>
@@ -6164,7 +6178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="71"/>
       <c r="B3" s="72"/>
       <c r="C3" s="8" t="s">
@@ -6199,7 +6213,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="71"/>
       <c r="B4" s="72"/>
       <c r="C4" s="8" t="s">
@@ -6219,7 +6233,7 @@
       </c>
       <c r="I4" s="71"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="71"/>
       <c r="B5" s="72"/>
       <c r="C5" s="9" t="s">
@@ -6239,19 +6253,19 @@
       </c>
       <c r="I5" s="71"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="71"/>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
       <c r="I6" s="71"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="71"/>
       <c r="B7" s="72" t="s">
         <v>115</v>
@@ -6276,7 +6290,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="71"/>
       <c r="B8" s="72"/>
       <c r="C8" s="15" t="s">
@@ -6311,7 +6325,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="71"/>
       <c r="B9" s="72"/>
       <c r="C9" s="8" t="s">
@@ -6331,7 +6345,7 @@
       </c>
       <c r="I9" s="71"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="71"/>
       <c r="B10" s="72"/>
       <c r="C10" s="9" t="s">
@@ -6351,17 +6365,17 @@
       </c>
       <c r="I10" s="71"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="71"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
       <c r="I11" s="71"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="71"/>
       <c r="B12" s="75" t="s">
         <v>117</v>
@@ -6398,7 +6412,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="71"/>
       <c r="B13" s="75"/>
       <c r="C13" s="15" t="s">
@@ -6433,7 +6447,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="71"/>
       <c r="B14" s="75"/>
       <c r="C14" s="9" t="s">
@@ -6458,7 +6472,7 @@
       <c r="M14" s="22"/>
       <c r="N14" s="23"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="71"/>
       <c r="B15" s="76"/>
       <c r="C15" s="9" t="s">
@@ -6493,7 +6507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="71"/>
       <c r="B16" s="73"/>
       <c r="C16" s="74"/>
@@ -6503,9 +6517,9 @@
       <c r="G16" s="74"/>
       <c r="I16" s="71"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="71"/>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="59" t="s">
         <v>113</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -6525,7 +6539,7 @@
       </c>
       <c r="I17" s="71"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" s="71"/>
       <c r="B18" s="75"/>
       <c r="C18" s="8" t="s">
@@ -6545,7 +6559,7 @@
       </c>
       <c r="I18" s="71"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="71"/>
       <c r="B19" s="75"/>
       <c r="C19" s="9" t="s">
@@ -6580,7 +6594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" s="71"/>
       <c r="B20" s="75"/>
       <c r="C20" s="15" t="s">
@@ -6615,7 +6629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21" s="71"/>
       <c r="B21" s="75"/>
       <c r="C21" s="9" t="s">
@@ -6640,7 +6654,7 @@
       <c r="M21" s="22"/>
       <c r="N21" s="23"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22" s="71"/>
       <c r="B22" s="76"/>
       <c r="C22" s="9" t="s">

</xml_diff>